<commit_message>
pso - mvo till 8 jan2016-7jan2021
</commit_message>
<xml_diff>
--- a/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
+++ b/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
   <si>
     <t xml:space="preserve">Date range</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t xml:space="preserve">7-Jan-2016 :: 6-Jan-2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8-Jan-2016 :: 7-Jan-2021</t>
   </si>
 </sst>
 </file>
@@ -395,10 +398,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD36"/>
+  <dimension ref="A1:AD43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3025,8 +3028,382 @@
         <v>33</v>
       </c>
     </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>29.3835376580014</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>17.719533768604</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>1.45621989804951</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>2.8401587000681</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <v>6.9628007630853</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>4.28442043112754</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <v>2.55465963998268</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>7.82061704303467</v>
+      </c>
+      <c r="L38" s="0" t="n">
+        <v>0.14935983281798</v>
+      </c>
+      <c r="M38" s="0" t="n">
+        <v>9.04523013960718</v>
+      </c>
+      <c r="N38" s="0" t="n">
+        <v>2.4605414793341</v>
+      </c>
+      <c r="O38" s="0" t="n">
+        <v>2.63691518133205</v>
+      </c>
+      <c r="P38" s="0" t="n">
+        <v>5.35161980724609</v>
+      </c>
+      <c r="Q38" s="0" t="n">
+        <v>1.11909785347891</v>
+      </c>
+      <c r="R38" s="0" t="n">
+        <v>5.92994158749161</v>
+      </c>
+      <c r="S38" s="0" t="n">
+        <v>2.38766071009967</v>
+      </c>
+      <c r="T38" s="0" t="n">
+        <v>1.45926160769788</v>
+      </c>
+      <c r="U38" s="0" t="n">
+        <v>3.74434555777137</v>
+      </c>
+      <c r="V38" s="0" t="n">
+        <v>0.915351208217588</v>
+      </c>
+      <c r="W38" s="0" t="n">
+        <v>9.44395587802283</v>
+      </c>
+      <c r="X38" s="0" t="n">
+        <v>8.46058118583972</v>
+      </c>
+      <c r="Y38" s="0" t="n">
+        <v>7.66256398312449</v>
+      </c>
+      <c r="Z38" s="0" t="n">
+        <v>0.1665872738048</v>
+      </c>
+      <c r="AA38" s="0" t="n">
+        <v>0.603758506956849</v>
+      </c>
+      <c r="AB38" s="0" t="n">
+        <v>6.65280735056821</v>
+      </c>
+      <c r="AC38" s="0" t="n">
+        <v>1.92775944360194</v>
+      </c>
+      <c r="AD38" s="0" t="n">
+        <v>5.42000483568845</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>30.5268165699694</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>11.616707475663</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>2.31966042240653</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>6.02249276516474</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>8.47720223096306</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>4.85283424798499</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>3.84056855186565</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>2.49153965834089</v>
+      </c>
+      <c r="L39" s="0" t="n">
+        <v>0.670632756246172</v>
+      </c>
+      <c r="M39" s="0" t="n">
+        <v>1.24747858990165</v>
+      </c>
+      <c r="N39" s="0" t="n">
+        <v>5.4704593694528</v>
+      </c>
+      <c r="O39" s="0" t="n">
+        <v>4.32524387709977</v>
+      </c>
+      <c r="P39" s="0" t="n">
+        <v>7.48709105822475</v>
+      </c>
+      <c r="Q39" s="0" t="n">
+        <v>0.707589925219238</v>
+      </c>
+      <c r="R39" s="0" t="n">
+        <v>2.0487872696163</v>
+      </c>
+      <c r="S39" s="0" t="n">
+        <v>4.04848964341325</v>
+      </c>
+      <c r="T39" s="0" t="n">
+        <v>0.0904522709183136</v>
+      </c>
+      <c r="U39" s="0" t="n">
+        <v>8.08381615795677</v>
+      </c>
+      <c r="V39" s="0" t="n">
+        <v>3.96798421868443</v>
+      </c>
+      <c r="W39" s="0" t="n">
+        <v>8.79700208858593</v>
+      </c>
+      <c r="X39" s="0" t="n">
+        <v>4.9705888829398</v>
+      </c>
+      <c r="Y39" s="0" t="n">
+        <v>6.41866648844545</v>
+      </c>
+      <c r="Z39" s="0" t="n">
+        <v>4.60116072087233</v>
+      </c>
+      <c r="AA39" s="0" t="n">
+        <v>0.518750740424009</v>
+      </c>
+      <c r="AB39" s="0" t="n">
+        <v>7.9360813274762</v>
+      </c>
+      <c r="AC39" s="0" t="n">
+        <v>0.867491217557508</v>
+      </c>
+      <c r="AD39" s="0" t="n">
+        <v>2.05759594264602</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3"/>
+      <c r="B40" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>28.8</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>17.8885438199983</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>1.40984085981362</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>0.227509410207713</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>11.7399060855447</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>0.580882923558929</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>8.96588452417452</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>2.93697282019851</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <v>2.09668392109204</v>
+      </c>
+      <c r="M40" s="0" t="n">
+        <v>8.82697051487464</v>
+      </c>
+      <c r="N40" s="0" t="n">
+        <v>18.5455319755054</v>
+      </c>
+      <c r="O40" s="0" t="n">
+        <v>0.961675586014997</v>
+      </c>
+      <c r="P40" s="0" t="n">
+        <v>7.71002905358488</v>
+      </c>
+      <c r="Q40" s="0" t="n">
+        <v>0.129010244836969</v>
+      </c>
+      <c r="R40" s="0" t="n">
+        <v>0.0133902191114465</v>
+      </c>
+      <c r="S40" s="0" t="n">
+        <v>2.93204243887695</v>
+      </c>
+      <c r="T40" s="0" t="n">
+        <v>4.10046519946671</v>
+      </c>
+      <c r="U40" s="0" t="n">
+        <v>7.69847090485439</v>
+      </c>
+      <c r="V40" s="0" t="n">
+        <v>1.4748551806485</v>
+      </c>
+      <c r="W40" s="0" t="n">
+        <v>0.348560308015893</v>
+      </c>
+      <c r="X40" s="0" t="n">
+        <v>4.12033278602222</v>
+      </c>
+      <c r="Y40" s="0" t="n">
+        <v>1.75960121490938</v>
+      </c>
+      <c r="Z40" s="0" t="n">
+        <v>0.292881170523793</v>
+      </c>
+      <c r="AA40" s="0" t="n">
+        <v>1.06304360597416</v>
+      </c>
+      <c r="AB40" s="0" t="n">
+        <v>11.5268607735217</v>
+      </c>
+      <c r="AC40" s="0" t="n">
+        <v>1.09245161713521</v>
+      </c>
+      <c r="AD40" s="0" t="n">
+        <v>0.855987521346332</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>30.2</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>11.6275534829989</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>2.28938959850171</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>2.6569208667856</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>7.45181052796176</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>10.7459695601984</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>2.44797199903069</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>1.3023077053619</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <v>5.11600331728191</v>
+      </c>
+      <c r="M41" s="0" t="n">
+        <v>6.99989873158132</v>
+      </c>
+      <c r="N41" s="0" t="n">
+        <v>0.972635935450368</v>
+      </c>
+      <c r="O41" s="0" t="n">
+        <v>1.90716900911576</v>
+      </c>
+      <c r="P41" s="0" t="n">
+        <v>17.3964788549832</v>
+      </c>
+      <c r="Q41" s="0" t="n">
+        <v>0.348705270320119</v>
+      </c>
+      <c r="R41" s="0" t="n">
+        <v>1.07274093988888</v>
+      </c>
+      <c r="S41" s="0" t="n">
+        <v>0.648931748930941</v>
+      </c>
+      <c r="T41" s="0" t="n">
+        <v>3.47701687007473</v>
+      </c>
+      <c r="U41" s="0" t="n">
+        <v>9.44086922459458</v>
+      </c>
+      <c r="V41" s="0" t="n">
+        <v>0.889158989965562</v>
+      </c>
+      <c r="W41" s="0" t="n">
+        <v>0.299414480173068</v>
+      </c>
+      <c r="X41" s="0" t="n">
+        <v>0.226735822947277</v>
+      </c>
+      <c r="Y41" s="0" t="n">
+        <v>7.64815173670969</v>
+      </c>
+      <c r="Z41" s="0" t="n">
+        <v>1.12874807800403</v>
+      </c>
+      <c r="AA41" s="0" t="n">
+        <v>0.612597631014368</v>
+      </c>
+      <c r="AB41" s="0" t="n">
+        <v>14.2502716919244</v>
+      </c>
+      <c r="AC41" s="0" t="n">
+        <v>0.630450079369199</v>
+      </c>
+      <c r="AD41" s="0" t="n">
+        <v>2.3290409283321</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3"/>
+      <c r="B42" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="24">
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B5"/>
@@ -3047,6 +3424,10 @@
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
update ACo hyps and pso hyps
karthik taking over from here
</commit_message>
<xml_diff>
--- a/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
+++ b/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="day sliding" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="hyperparameters" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="hyperparameterACOs" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="PSOhyps" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -180,7 +181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -209,11 +210,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -301,7 +297,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -354,11 +350,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -441,7 +433,7 @@
   </sheetPr>
   <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -5107,7 +5099,7 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -5136,7 +5128,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -5145,7 +5137,7 @@
       <c r="C6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="14" t="n">
+      <c r="D6" s="13" t="n">
         <v>1.4165359383584</v>
       </c>
       <c r="E6" s="1" t="n">
@@ -5162,7 +5154,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13"/>
+      <c r="A7" s="3"/>
       <c r="B7" s="10"/>
       <c r="C7" s="9" t="s">
         <v>33</v>
@@ -5187,7 +5179,7 @@
       <c r="A8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -5213,7 +5205,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13"/>
+      <c r="A10" s="3"/>
       <c r="B10" s="10"/>
       <c r="C10" s="9" t="s">
         <v>33</v>
@@ -5235,7 +5227,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -5246,14 +5238,14 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13"/>
+      <c r="A13" s="3"/>
       <c r="B13" s="10"/>
       <c r="C13" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -5279,7 +5271,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13"/>
+      <c r="A16" s="3"/>
       <c r="B16" s="10"/>
       <c r="C16" s="9" t="s">
         <v>33</v>
@@ -5301,7 +5293,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -5327,7 +5319,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13"/>
+      <c r="A19" s="3"/>
       <c r="B19" s="10"/>
       <c r="C19" s="9" t="s">
         <v>33</v>
@@ -5349,7 +5341,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -5360,14 +5352,14 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13"/>
+      <c r="A22" s="3"/>
       <c r="B22" s="10"/>
       <c r="C22" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -5393,7 +5385,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13"/>
+      <c r="A25" s="3"/>
       <c r="B25" s="10"/>
       <c r="C25" s="9" t="s">
         <v>33</v>
@@ -5439,4 +5431,27 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
20jan and 21jan outputs and edits
</commit_message>
<xml_diff>
--- a/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
+++ b/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="58">
   <si>
     <t>Date range</t>
   </si>
@@ -190,6 +190,12 @@
   <si>
     <t>19-Jan-2016 ::18-Jan-2021</t>
   </si>
+  <si>
+    <t>20-Jan-2016 ::19-Jan-2021</t>
+  </si>
+  <si>
+    <t>21-Jan-2016 ::20-Jan-2021</t>
+  </si>
 </sst>
 </file>
 
@@ -280,21 +286,6 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -322,10 +313,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,120 +694,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMJ98"/>
+  <dimension ref="A1:AMJ114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110:AD110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="6" style="6" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="6" customWidth="1"/>
-    <col min="4" max="1024" width="11.5703125" style="6"/>
+    <col min="1" max="1" width="9.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="1" customWidth="1"/>
+    <col min="4" max="1024" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="25.5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D2">
@@ -887,9 +893,9 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="25.5">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="10" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D3">
@@ -975,358 +981,358 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="1">
         <v>33.4</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="1">
         <v>20.124611797498101</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="1">
         <v>1.4817677130898601</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="1">
         <v>7.9527390977652795E-2</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="1">
         <v>22.4464268497482</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="1">
         <v>0.25733436844476199</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="1">
         <v>0.83970564615458798</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="1">
         <v>13.769638687008801</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="1">
         <v>0.77676813194347905</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="1">
         <v>13.266950941268</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="1">
         <v>3.12185935387879</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="1">
         <v>3.9137542296357103E-2</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="1">
         <v>8.0993263709179999</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="Q4" s="1">
         <v>7.7609373197022801E-3</v>
       </c>
-      <c r="R4" s="6">
+      <c r="R4" s="1">
         <v>0.115734468143942</v>
       </c>
-      <c r="S4" s="6">
+      <c r="S4" s="1">
         <v>0.700010545353425</v>
       </c>
-      <c r="T4" s="6">
+      <c r="T4" s="1">
         <v>0.47170903446363799</v>
       </c>
-      <c r="U4" s="6">
+      <c r="U4" s="1">
         <v>9.1639014261746699</v>
       </c>
-      <c r="V4" s="6">
+      <c r="V4" s="1">
         <v>0.64429754029554298</v>
       </c>
-      <c r="W4" s="6">
+      <c r="W4" s="1">
         <v>5.2811712317144301E-2</v>
       </c>
-      <c r="X4" s="6">
+      <c r="X4" s="1">
         <v>0.38361573795180398</v>
       </c>
-      <c r="Y4" s="6">
+      <c r="Y4" s="1">
         <v>3.6131235674055402</v>
       </c>
-      <c r="Z4" s="6">
+      <c r="Z4" s="1">
         <v>5.8078805284563702</v>
       </c>
-      <c r="AA4" s="6">
+      <c r="AA4" s="1">
         <v>1.47507561034199</v>
       </c>
-      <c r="AB4" s="6">
+      <c r="AB4" s="1">
         <v>13.2410058761967</v>
       </c>
-      <c r="AC4" s="6">
+      <c r="AC4" s="1">
         <v>0.22518442267864999</v>
       </c>
-      <c r="AD4" s="6">
+      <c r="AD4" s="1">
         <v>1.4012133102623301</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="25.5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="12" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="1">
         <v>28.2</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="1">
         <v>10.733126291999</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="1">
         <v>2.2938330669185301</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="1">
         <v>1.6543985476799901</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="1">
         <v>3.2713886671087199E-6</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="1">
         <v>8.7072622339152606</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="1">
         <v>6.9307411612482203E-3</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="1">
         <v>0.31145953095198697</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="1">
         <v>3.6065607324878901E-2</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="1">
         <v>13.8390635904781</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="1">
         <v>2.9005036469138301</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="1">
         <v>4.2643679960571397E-2</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="1">
         <v>0.195213362114255</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="1">
         <v>0.27091926316542903</v>
       </c>
-      <c r="R5" s="6">
+      <c r="R5" s="1">
         <v>5.5659362995075495E-4</v>
       </c>
-      <c r="S5" s="6">
+      <c r="S5" s="1">
         <v>8.9691427777364204E-4</v>
       </c>
-      <c r="T5" s="6">
+      <c r="T5" s="1">
         <v>2.55930242767771E-2</v>
       </c>
-      <c r="U5" s="6">
+      <c r="U5" s="1">
         <v>42.2484109538347</v>
       </c>
-      <c r="V5" s="6">
+      <c r="V5" s="1">
         <v>5.5568725371925698</v>
       </c>
-      <c r="W5" s="6">
+      <c r="W5" s="1">
         <v>4.7830986438024201</v>
       </c>
-      <c r="X5" s="6">
+      <c r="X5" s="1">
         <v>1.9062865557336</v>
       </c>
-      <c r="Y5" s="6">
+      <c r="Y5" s="1">
         <v>17.2813893591191</v>
       </c>
-      <c r="Z5" s="6">
+      <c r="Z5" s="1">
         <v>1.32904759460731E-4</v>
       </c>
-      <c r="AA5" s="6">
+      <c r="AA5" s="1">
         <v>5.0356109210957102E-2</v>
       </c>
-      <c r="AB5" s="6">
+      <c r="AB5" s="1">
         <v>0.12957429879380999</v>
       </c>
-      <c r="AC5" s="6">
+      <c r="AC5" s="1">
         <v>1.8982271340490402E-2</v>
       </c>
-      <c r="AD5" s="6">
+      <c r="AD5" s="1">
         <v>3.33863589740876E-2</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="8">
         <v>0.27900471696332502</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="8">
         <v>0.181111190804886</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="8">
         <v>1.3428475395832</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="8">
         <v>2.79233758435109E-2</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="8">
         <v>5.8845780195611402E-2</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="8">
         <v>4.8538312078244598E-2</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="8">
         <v>7.9460716430344996E-2</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="8">
         <v>5.8845780195611402E-2</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="8">
         <v>1.24621736674607E-2</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="8">
         <v>1.24621736674607E-2</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="8">
         <v>7.9460716430344996E-2</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="8">
         <v>5.3692046136927997E-2</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6" s="8">
         <v>6.3999514254294801E-2</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="8">
         <v>7.3084396087772603E-3</v>
       </c>
-      <c r="R6" s="13">
+      <c r="R6" s="8">
         <v>6.3999514254294801E-2</v>
       </c>
-      <c r="S6" s="13">
+      <c r="S6" s="8">
         <v>4.3384578019561103E-2</v>
       </c>
-      <c r="T6" s="13">
+      <c r="T6" s="8">
         <v>3.3077109902194299E-2</v>
       </c>
-      <c r="U6" s="13">
+      <c r="U6" s="8">
         <v>6.9153248312978199E-2</v>
       </c>
-      <c r="V6" s="13">
+      <c r="V6" s="8">
         <v>1.24621736674607E-2</v>
       </c>
-      <c r="W6" s="13">
+      <c r="W6" s="8">
         <v>5.8845780195611402E-2</v>
       </c>
-      <c r="X6" s="13">
+      <c r="X6" s="8">
         <v>5.3692046136927997E-2</v>
       </c>
-      <c r="Y6" s="13">
+      <c r="Y6" s="8">
         <v>6.9153248312978199E-2</v>
       </c>
-      <c r="Z6" s="13">
+      <c r="Z6" s="8">
         <v>1.24621736674607E-2</v>
       </c>
-      <c r="AA6" s="13">
+      <c r="AA6" s="8">
         <v>3.8230843960877697E-2</v>
       </c>
-      <c r="AB6" s="13">
+      <c r="AB6" s="8">
         <v>7.3084396087772603E-3</v>
       </c>
-      <c r="AC6" s="13">
+      <c r="AC6" s="8">
         <v>2.2769641784827498E-2</v>
       </c>
-      <c r="AD6" s="13">
+      <c r="AD6" s="8">
         <v>1.24621736674607E-2</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="25.5">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="12" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="8">
         <v>0.28067536281093403</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="8">
         <v>0.115338965607968</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="8">
         <v>2.1230931066544598</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="8">
         <v>5.5559440002794398E-2</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="8">
         <v>7.0056246962232102E-2</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="8">
         <v>7.2367501380021697E-3</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="8">
         <v>3.6230364056877497E-2</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="8">
         <v>7.4888515948711404E-2</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="8">
         <v>1.6901288110960599E-2</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="8">
         <v>7.2367501380021697E-3</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="8">
         <v>7.0056246962232102E-2</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="8">
         <v>3.6230364056877497E-2</v>
       </c>
-      <c r="P7" s="13">
+      <c r="P7" s="8">
         <v>5.5559440002794398E-2</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="Q7" s="8">
         <v>3.1398095070398299E-2</v>
       </c>
-      <c r="R7" s="13">
+      <c r="R7" s="8">
         <v>7.0056246962232102E-2</v>
       </c>
-      <c r="S7" s="13">
+      <c r="S7" s="8">
         <v>3.1398095070398299E-2</v>
       </c>
-      <c r="T7" s="13">
+      <c r="T7" s="8">
         <v>1.6901288110960599E-2</v>
       </c>
-      <c r="U7" s="13">
+      <c r="U7" s="8">
         <v>6.03917089892737E-2</v>
       </c>
-      <c r="V7" s="13">
+      <c r="V7" s="8">
         <v>1.6901288110960599E-2</v>
       </c>
-      <c r="W7" s="13">
+      <c r="W7" s="8">
         <v>1.6901288110960599E-2</v>
       </c>
-      <c r="X7" s="13">
+      <c r="X7" s="8">
         <v>3.1398095070398299E-2</v>
       </c>
-      <c r="Y7" s="13">
+      <c r="Y7" s="8">
         <v>6.03917089892737E-2</v>
       </c>
-      <c r="Z7" s="13">
+      <c r="Z7" s="8">
         <v>4.5894902029836003E-2</v>
       </c>
-      <c r="AA7" s="13">
+      <c r="AA7" s="8">
         <v>5.5559440002794398E-2</v>
       </c>
-      <c r="AB7" s="13">
+      <c r="AB7" s="8">
         <v>7.4888515948711404E-2</v>
       </c>
-      <c r="AC7" s="13">
+      <c r="AC7" s="8">
         <v>4.5894902029836003E-2</v>
       </c>
-      <c r="AD7" s="13">
+      <c r="AD7" s="8">
         <v>1.2069019124481399E-2</v>
       </c>
     </row>
@@ -1336,13 +1342,13 @@
       <c r="C8"/>
     </row>
     <row r="9" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D9">
@@ -1428,9 +1434,9 @@
       </c>
     </row>
     <row r="10" spans="1:30" ht="25.5">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="12" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D10">
@@ -1516,11 +1522,11 @@
       </c>
     </row>
     <row r="11" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D11">
@@ -1606,9 +1612,9 @@
       </c>
     </row>
     <row r="12" spans="1:30" ht="25.5">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="12" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D12">
@@ -1694,11 +1700,11 @@
       </c>
     </row>
     <row r="13" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D13">
@@ -1784,9 +1790,9 @@
       </c>
     </row>
     <row r="14" spans="1:30" ht="25.5">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="12" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D14">
@@ -1872,13 +1878,13 @@
       </c>
     </row>
     <row r="16" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D16">
@@ -1964,9 +1970,9 @@
       </c>
     </row>
     <row r="17" spans="1:30" ht="25.5">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="12" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D17">
@@ -2052,11 +2058,11 @@
       </c>
     </row>
     <row r="18" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D18">
@@ -2142,9 +2148,9 @@
       </c>
     </row>
     <row r="19" spans="1:30" ht="25.5">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="12" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D19">
@@ -2230,11 +2236,11 @@
       </c>
     </row>
     <row r="20" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A20" s="5"/>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="12"/>
+      <c r="B20" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D20">
@@ -2320,9 +2326,9 @@
       </c>
     </row>
     <row r="21" spans="1:30" ht="25.5">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="12" t="s">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D21">
@@ -2409,13 +2415,13 @@
     </row>
     <row r="22" spans="1:30" ht="40.5" customHeight="1"/>
     <row r="23" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D23">
@@ -2501,9 +2507,9 @@
       </c>
     </row>
     <row r="24" spans="1:30" ht="25.5">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="12" t="s">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D24">
@@ -2589,11 +2595,11 @@
       </c>
     </row>
     <row r="25" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A25" s="5"/>
-      <c r="B25" s="3" t="s">
+      <c r="A25" s="12"/>
+      <c r="B25" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D25">
@@ -2679,9 +2685,9 @@
       </c>
     </row>
     <row r="26" spans="1:30" ht="25.5">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="12" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D26">
@@ -2767,11 +2773,11 @@
       </c>
     </row>
     <row r="27" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A27" s="5"/>
-      <c r="B27" s="2" t="s">
+      <c r="A27" s="12"/>
+      <c r="B27" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D27">
@@ -2857,9 +2863,9 @@
       </c>
     </row>
     <row r="28" spans="1:30" ht="25.5">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="12" t="s">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D28">
@@ -2945,13 +2951,13 @@
       </c>
     </row>
     <row r="31" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D31">
@@ -3037,9 +3043,9 @@
       </c>
     </row>
     <row r="32" spans="1:30" ht="25.5">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="12" t="s">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D32">
@@ -3125,11 +3131,11 @@
       </c>
     </row>
     <row r="33" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A33" s="5"/>
-      <c r="B33" s="3" t="s">
+      <c r="A33" s="12"/>
+      <c r="B33" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D33">
@@ -3215,9 +3221,9 @@
       </c>
     </row>
     <row r="34" spans="1:30" ht="25.5">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="12" t="s">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D34">
@@ -3303,11 +3309,11 @@
       </c>
     </row>
     <row r="35" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A35" s="5"/>
-      <c r="B35" s="2" t="s">
+      <c r="A35" s="12"/>
+      <c r="B35" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D35">
@@ -3393,9 +3399,9 @@
       </c>
     </row>
     <row r="36" spans="1:30" ht="25.5">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="12" t="s">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D36">
@@ -3481,13 +3487,13 @@
       </c>
     </row>
     <row r="38" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D38">
@@ -3573,9 +3579,9 @@
       </c>
     </row>
     <row r="39" spans="1:30" ht="25.5">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="12" t="s">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D39">
@@ -3661,11 +3667,11 @@
       </c>
     </row>
     <row r="40" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A40" s="5"/>
-      <c r="B40" s="3" t="s">
+      <c r="A40" s="12"/>
+      <c r="B40" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D40">
@@ -3751,9 +3757,9 @@
       </c>
     </row>
     <row r="41" spans="1:30" ht="25.5">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="12" t="s">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D41">
@@ -3839,11 +3845,11 @@
       </c>
     </row>
     <row r="42" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A42" s="5"/>
-      <c r="B42" s="2" t="s">
+      <c r="A42" s="12"/>
+      <c r="B42" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D42">
@@ -3929,9 +3935,9 @@
       </c>
     </row>
     <row r="43" spans="1:30" ht="25.5">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="12" t="s">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D43">
@@ -4017,13 +4023,13 @@
       </c>
     </row>
     <row r="46" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D46">
@@ -4109,9 +4115,9 @@
       </c>
     </row>
     <row r="47" spans="1:30" ht="25.5">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="12" t="s">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D47">
@@ -4197,11 +4203,11 @@
       </c>
     </row>
     <row r="48" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A48" s="5"/>
-      <c r="B48" s="3" t="s">
+      <c r="A48" s="12"/>
+      <c r="B48" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D48">
@@ -4287,9 +4293,9 @@
       </c>
     </row>
     <row r="49" spans="1:30" ht="25.5">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="12" t="s">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D49">
@@ -4375,11 +4381,11 @@
       </c>
     </row>
     <row r="50" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A50" s="5"/>
-      <c r="B50" s="2" t="s">
+      <c r="A50" s="12"/>
+      <c r="B50" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D50">
@@ -4465,9 +4471,9 @@
       </c>
     </row>
     <row r="51" spans="1:30" ht="25.5">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="12" t="s">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D51">
@@ -4553,13 +4559,13 @@
       </c>
     </row>
     <row r="54" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D54">
@@ -4645,9 +4651,9 @@
       </c>
     </row>
     <row r="55" spans="1:30" ht="25.5">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="12" t="s">
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D55">
@@ -4733,11 +4739,11 @@
       </c>
     </row>
     <row r="56" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A56" s="5"/>
-      <c r="B56" s="3" t="s">
+      <c r="A56" s="12"/>
+      <c r="B56" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D56">
@@ -4823,9 +4829,9 @@
       </c>
     </row>
     <row r="57" spans="1:30" ht="25.5">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="12" t="s">
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D57">
@@ -4911,11 +4917,11 @@
       </c>
     </row>
     <row r="58" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A58" s="5"/>
-      <c r="B58" s="2" t="s">
+      <c r="A58" s="12"/>
+      <c r="B58" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D58">
@@ -5001,9 +5007,9 @@
       </c>
     </row>
     <row r="59" spans="1:30" ht="25.5">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="12" t="s">
+      <c r="A59" s="12"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D59">
@@ -5089,13 +5095,13 @@
       </c>
     </row>
     <row r="62" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D62">
@@ -5181,9 +5187,9 @@
       </c>
     </row>
     <row r="63" spans="1:30" ht="25.5">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="12" t="s">
+      <c r="A63" s="12"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D63">
@@ -5269,11 +5275,11 @@
       </c>
     </row>
     <row r="64" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A64" s="5"/>
-      <c r="B64" s="3" t="s">
+      <c r="A64" s="12"/>
+      <c r="B64" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C64" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D64">
@@ -5359,9 +5365,9 @@
       </c>
     </row>
     <row r="65" spans="1:30" ht="25.5">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="12" t="s">
+      <c r="A65" s="12"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D65">
@@ -5447,11 +5453,11 @@
       </c>
     </row>
     <row r="66" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A66" s="5"/>
-      <c r="B66" s="2" t="s">
+      <c r="A66" s="12"/>
+      <c r="B66" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D66">
@@ -5537,9 +5543,9 @@
       </c>
     </row>
     <row r="67" spans="1:30" ht="25.5">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="12" t="s">
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D67">
@@ -5625,13 +5631,13 @@
       </c>
     </row>
     <row r="70" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="C70" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D70">
@@ -5717,9 +5723,9 @@
       </c>
     </row>
     <row r="71" spans="1:30" ht="25.5">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="12" t="s">
+      <c r="A71" s="12"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D71">
@@ -5805,11 +5811,11 @@
       </c>
     </row>
     <row r="72" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A72" s="5"/>
-      <c r="B72" s="3" t="s">
+      <c r="A72" s="12"/>
+      <c r="B72" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D72">
@@ -5895,9 +5901,9 @@
       </c>
     </row>
     <row r="73" spans="1:30" ht="25.5">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="12" t="s">
+      <c r="A73" s="12"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D73">
@@ -5983,11 +5989,11 @@
       </c>
     </row>
     <row r="74" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A74" s="5"/>
-      <c r="B74" s="2" t="s">
+      <c r="A74" s="12"/>
+      <c r="B74" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D74">
@@ -6073,9 +6079,9 @@
       </c>
     </row>
     <row r="75" spans="1:30" ht="25.5">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="12" t="s">
+      <c r="A75" s="12"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D75">
@@ -6161,13 +6167,13 @@
       </c>
     </row>
     <row r="78" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D78">
@@ -6253,9 +6259,9 @@
       </c>
     </row>
     <row r="79" spans="1:30" ht="25.5">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="12" t="s">
+      <c r="A79" s="12"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D79">
@@ -6341,11 +6347,11 @@
       </c>
     </row>
     <row r="80" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A80" s="5"/>
-      <c r="B80" s="3" t="s">
+      <c r="A80" s="12"/>
+      <c r="B80" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C80" s="11" t="s">
+      <c r="C80" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D80">
@@ -6431,9 +6437,9 @@
       </c>
     </row>
     <row r="81" spans="1:30" ht="25.5">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
-      <c r="C81" s="12" t="s">
+      <c r="A81" s="12"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D81">
@@ -6519,11 +6525,11 @@
       </c>
     </row>
     <row r="82" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A82" s="5"/>
-      <c r="B82" s="2" t="s">
+      <c r="A82" s="12"/>
+      <c r="B82" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C82" s="11" t="s">
+      <c r="C82" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D82">
@@ -6609,9 +6615,9 @@
       </c>
     </row>
     <row r="83" spans="1:30" ht="25.5">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="12" t="s">
+      <c r="A83" s="12"/>
+      <c r="B83" s="12"/>
+      <c r="C83" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D83">
@@ -6697,13 +6703,13 @@
       </c>
     </row>
     <row r="85" spans="1:30" ht="25.5">
-      <c r="A85" s="15" t="s">
+      <c r="A85" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C85" s="11" t="s">
+      <c r="C85" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D85">
@@ -6789,9 +6795,9 @@
       </c>
     </row>
     <row r="86" spans="1:30" ht="25.5">
-      <c r="A86" s="5"/>
-      <c r="B86" s="5"/>
-      <c r="C86" s="12" t="s">
+      <c r="A86" s="12"/>
+      <c r="B86" s="12"/>
+      <c r="C86" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D86">
@@ -6877,11 +6883,11 @@
       </c>
     </row>
     <row r="87" spans="1:30" ht="25.5">
-      <c r="A87" s="5"/>
-      <c r="B87" s="3" t="s">
+      <c r="A87" s="12"/>
+      <c r="B87" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="C87" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D87">
@@ -6911,10 +6917,10 @@
       <c r="L87">
         <v>1.7261854900860199E-4</v>
       </c>
-      <c r="M87" s="16">
+      <c r="M87" s="10">
         <v>1.0124585088725201E-5</v>
       </c>
-      <c r="N87" s="16">
+      <c r="N87" s="10">
         <v>5.6864110624996702E-7</v>
       </c>
       <c r="O87">
@@ -6938,7 +6944,7 @@
       <c r="U87">
         <v>1.3408169013852099E-4</v>
       </c>
-      <c r="V87" s="16">
+      <c r="V87" s="10">
         <v>1.9902616833019301E-5</v>
       </c>
       <c r="W87">
@@ -6967,9 +6973,9 @@
       </c>
     </row>
     <row r="88" spans="1:30" ht="25.5">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
-      <c r="C88" s="12" t="s">
+      <c r="A88" s="12"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D88">
@@ -7055,11 +7061,11 @@
       </c>
     </row>
     <row r="89" spans="1:30" ht="25.5">
-      <c r="A89" s="5"/>
-      <c r="B89" s="2" t="s">
+      <c r="A89" s="12"/>
+      <c r="B89" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C89" s="11" t="s">
+      <c r="C89" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D89">
@@ -7145,9 +7151,9 @@
       </c>
     </row>
     <row r="90" spans="1:30" ht="25.5">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="12" t="s">
+      <c r="A90" s="12"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D90">
@@ -7233,13 +7239,13 @@
       </c>
     </row>
     <row r="93" spans="1:30" ht="25.5">
-      <c r="A93" s="15" t="s">
+      <c r="A93" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="C93" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D93">
@@ -7325,9 +7331,9 @@
       </c>
     </row>
     <row r="94" spans="1:30" ht="25.5">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="12" t="s">
+      <c r="A94" s="12"/>
+      <c r="B94" s="12"/>
+      <c r="C94" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D94">
@@ -7413,39 +7419,1159 @@
       </c>
     </row>
     <row r="95" spans="1:30" ht="25.5">
-      <c r="A95" s="5"/>
-      <c r="B95" s="3" t="s">
+      <c r="A95" s="12"/>
+      <c r="B95" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C95" s="11" t="s">
+      <c r="C95" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="D95">
+        <v>34.599999999999902</v>
+      </c>
+      <c r="E95">
+        <v>21.019038988498</v>
+      </c>
+      <c r="F95">
+        <v>1.4758048651498601</v>
+      </c>
+      <c r="G95">
+        <v>1.8624372415703E-2</v>
+      </c>
+      <c r="H95">
+        <v>26.574732397063499</v>
+      </c>
+      <c r="I95">
+        <v>1.0642866864477501E-2</v>
+      </c>
+      <c r="J95">
+        <v>9.8425728580171304E-2</v>
+      </c>
+      <c r="K95">
+        <v>0.64714693380153399</v>
+      </c>
+      <c r="L95">
+        <v>0.58735922253448203</v>
+      </c>
+      <c r="M95">
+        <v>4.8693836462651499</v>
+      </c>
+      <c r="N95">
+        <v>0.23103385401215601</v>
+      </c>
+      <c r="O95">
+        <v>0.54182349244976602</v>
+      </c>
+      <c r="P95">
+        <v>0.90980176391255096</v>
+      </c>
+      <c r="Q95">
+        <v>1.1420976764721601E-4</v>
+      </c>
+      <c r="R95">
+        <v>1.4271373894878401</v>
+      </c>
+      <c r="S95">
+        <v>1.2328382311372999E-2</v>
+      </c>
+      <c r="T95">
+        <v>0.15688771338631899</v>
+      </c>
+      <c r="U95">
+        <v>0.21137891415416901</v>
+      </c>
+      <c r="V95">
+        <v>0.72168996051406997</v>
+      </c>
+      <c r="W95">
+        <v>0.16773871226089099</v>
+      </c>
+      <c r="X95">
+        <v>37.816313046777402</v>
+      </c>
+      <c r="Y95">
+        <v>11.572186309022101</v>
+      </c>
+      <c r="Z95">
+        <v>5.61349685912267E-2</v>
+      </c>
+      <c r="AA95">
+        <v>1.6456501209032499</v>
+      </c>
+      <c r="AB95">
+        <v>8.7456218929471508</v>
+      </c>
+      <c r="AC95">
+        <v>2.0818187873892402</v>
+      </c>
+      <c r="AD95">
+        <v>0.89602531458769996</v>
+      </c>
     </row>
     <row r="96" spans="1:30" ht="25.5">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
-      <c r="C96" s="12" t="s">
+      <c r="A96" s="12"/>
+      <c r="B96" s="12"/>
+      <c r="C96" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" ht="25.5">
-      <c r="A97" s="5"/>
-      <c r="B97" s="2" t="s">
+      <c r="D96">
+        <v>30</v>
+      </c>
+      <c r="E96">
+        <v>11.180339887498899</v>
+      </c>
+      <c r="F96">
+        <v>2.3630766386217701</v>
+      </c>
+      <c r="G96">
+        <v>2.8078254364438502</v>
+      </c>
+      <c r="H96">
+        <v>1.3396619026711001</v>
+      </c>
+      <c r="I96">
+        <v>1.5317928657397899</v>
+      </c>
+      <c r="J96">
+        <v>1.6157573593254999</v>
+      </c>
+      <c r="K96">
+        <v>0.24887280090245001</v>
+      </c>
+      <c r="L96">
+        <v>0.66830887124129501</v>
+      </c>
+      <c r="M96">
+        <v>0.201325510862056</v>
+      </c>
+      <c r="N96">
+        <v>9.2153219079964301E-3</v>
+      </c>
+      <c r="O96">
+        <v>1.0149177049361799</v>
+      </c>
+      <c r="P96">
+        <v>27.396052478592399</v>
+      </c>
+      <c r="Q96">
+        <v>3.9963248402001203E-2</v>
+      </c>
+      <c r="R96">
+        <v>2.0109376159993602</v>
+      </c>
+      <c r="S96">
+        <v>18.176986713838598</v>
+      </c>
+      <c r="T96">
+        <v>0.57420352123853502</v>
+      </c>
+      <c r="U96">
+        <v>11.971758719101199</v>
+      </c>
+      <c r="V96">
+        <v>2.2231799092512201</v>
+      </c>
+      <c r="W96">
+        <v>11.3405657971492</v>
+      </c>
+      <c r="X96">
+        <v>2.6688506099090601E-2</v>
+      </c>
+      <c r="Y96">
+        <v>3.9292767654573599</v>
+      </c>
+      <c r="Z96">
+        <v>0.33411773839685099</v>
+      </c>
+      <c r="AA96">
+        <v>5.0652019084127801E-2</v>
+      </c>
+      <c r="AB96">
+        <v>10.127430010599999</v>
+      </c>
+      <c r="AC96">
+        <v>2.2863394897031002</v>
+      </c>
+      <c r="AD96">
+        <v>7.41696930564716E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:30" ht="25.5">
+      <c r="A97" s="12"/>
+      <c r="B97" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C97" s="11" t="s">
+      <c r="C97" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" ht="25.5">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5"/>
-      <c r="C98" s="12" t="s">
+      <c r="D97">
+        <v>28.308575968363101</v>
+      </c>
+      <c r="E97">
+        <v>17.475301331630199</v>
+      </c>
+      <c r="F97">
+        <v>141.50586304114</v>
+      </c>
+      <c r="G97">
+        <v>7.8999413391789997</v>
+      </c>
+      <c r="H97">
+        <v>7.3468636099179099</v>
+      </c>
+      <c r="I97">
+        <v>1.2630085880459601</v>
+      </c>
+      <c r="J97">
+        <v>6.7937858806568201</v>
+      </c>
+      <c r="K97">
+        <v>2.9222417758292201</v>
+      </c>
+      <c r="L97">
+        <v>5.6876304221346503</v>
+      </c>
+      <c r="M97">
+        <v>4.5814749636124796</v>
+      </c>
+      <c r="N97">
+        <v>2.3691640465681298</v>
+      </c>
+      <c r="O97">
+        <v>0.70993085878487405</v>
+      </c>
+      <c r="P97">
+        <v>5.6876304221346503</v>
+      </c>
+      <c r="Q97">
+        <v>2.3691640465681298</v>
+      </c>
+      <c r="R97">
+        <v>2.3691640465681298</v>
+      </c>
+      <c r="S97">
+        <v>2.3691640465681298</v>
+      </c>
+      <c r="T97">
+        <v>0.70993085878487405</v>
+      </c>
+      <c r="U97">
+        <v>1.8160863173070401</v>
+      </c>
+      <c r="V97">
+        <v>6.2407081513957401</v>
+      </c>
+      <c r="W97">
+        <v>7.3468636099179099</v>
+      </c>
+      <c r="X97">
+        <v>8.4530190684400903</v>
+      </c>
+      <c r="Y97">
+        <v>8.4530190684400903</v>
+      </c>
+      <c r="Z97">
+        <v>1.2630085880459601</v>
+      </c>
+      <c r="AA97">
+        <v>2.3691640465681298</v>
+      </c>
+      <c r="AB97">
+        <v>5.1345526928735596</v>
+      </c>
+      <c r="AC97">
+        <v>1.2630085880459601</v>
+      </c>
+      <c r="AD97">
+        <v>4.5814749636124796</v>
+      </c>
+    </row>
+    <row r="98" spans="1:30" ht="25.5">
+      <c r="A98" s="12"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="D98">
+        <v>28.192257268321502</v>
+      </c>
+      <c r="E98">
+        <v>11.054884989267601</v>
+      </c>
+      <c r="F98">
+        <v>222.63693645131201</v>
+      </c>
+      <c r="G98">
+        <v>6.7990506280679197</v>
+      </c>
+      <c r="H98">
+        <v>7.3484177156647101</v>
+      </c>
+      <c r="I98">
+        <v>0.75601266450329097</v>
+      </c>
+      <c r="J98">
+        <v>4.0522151900840004</v>
+      </c>
+      <c r="K98">
+        <v>5.1509493652775697</v>
+      </c>
+      <c r="L98">
+        <v>2.4041139272936398</v>
+      </c>
+      <c r="M98">
+        <v>6.7990506280679197</v>
+      </c>
+      <c r="N98">
+        <v>7.8977848032614997</v>
+      </c>
+      <c r="O98">
+        <v>1.8547468396968601</v>
+      </c>
+      <c r="P98">
+        <v>8.4471518908582794</v>
+      </c>
+      <c r="Q98">
+        <v>3.50284810248721</v>
+      </c>
+      <c r="R98">
+        <v>5.1509493652775697</v>
+      </c>
+      <c r="S98">
+        <v>2.4041139272936398</v>
+      </c>
+      <c r="T98">
+        <v>5.1509493652775697</v>
+      </c>
+      <c r="U98">
+        <v>4.0522151900840004</v>
+      </c>
+      <c r="V98">
+        <v>2.9534810148904298</v>
+      </c>
+      <c r="W98">
+        <v>3.50284810248721</v>
+      </c>
+      <c r="X98">
+        <v>3.50284810248721</v>
+      </c>
+      <c r="Y98">
+        <v>8.4471518908582794</v>
+      </c>
+      <c r="Z98">
+        <v>1.3053797521000701</v>
+      </c>
+      <c r="AA98">
+        <v>0.75601266450329097</v>
+      </c>
+      <c r="AB98">
+        <v>2.4041139272936398</v>
+      </c>
+      <c r="AC98">
+        <v>1.8547468396968601</v>
+      </c>
+      <c r="AD98">
+        <v>3.50284810248721</v>
+      </c>
+    </row>
+    <row r="101" spans="1:30" ht="25.5">
+      <c r="A101" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B101" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D101">
+        <v>29.428662673760801</v>
+      </c>
+      <c r="E101">
+        <v>17.139315168134701</v>
+      </c>
+      <c r="F101">
+        <v>1.50815026272569</v>
+      </c>
+      <c r="G101">
+        <v>7.22152890090097</v>
+      </c>
+      <c r="H101">
+        <v>7.6012345065165103</v>
+      </c>
+      <c r="I101">
+        <v>2.1592382382965498</v>
+      </c>
+      <c r="J101">
+        <v>4.0750520454607102</v>
+      </c>
+      <c r="K101">
+        <v>5.4049511325980797</v>
+      </c>
+      <c r="L101">
+        <v>1.1394118971587099</v>
+      </c>
+      <c r="M101">
+        <v>4.3496615466374999</v>
+      </c>
+      <c r="N101">
+        <v>3.23792232052228</v>
+      </c>
+      <c r="O101">
+        <v>0.53666809160256801</v>
+      </c>
+      <c r="P101">
+        <v>6.92956919071126</v>
+      </c>
+      <c r="Q101">
+        <v>2.19619952250327</v>
+      </c>
+      <c r="R101">
+        <v>7.8705074605868797</v>
+      </c>
+      <c r="S101">
+        <v>0.95859947953693003</v>
+      </c>
+      <c r="T101">
+        <v>0.68666019157685898</v>
+      </c>
+      <c r="U101">
+        <v>7.9521660032603698</v>
+      </c>
+      <c r="V101">
+        <v>5.8624506488922004</v>
+      </c>
+      <c r="W101">
+        <v>5.8730082157919297</v>
+      </c>
+      <c r="X101">
+        <v>4.7943282891268098</v>
+      </c>
+      <c r="Y101">
+        <v>5.6143134777887296</v>
+      </c>
+      <c r="Z101">
+        <v>1.90924489856045</v>
+      </c>
+      <c r="AA101">
+        <v>3.78780630190372</v>
+      </c>
+      <c r="AB101">
+        <v>7.7614400129287002</v>
+      </c>
+      <c r="AC101">
+        <v>1.46013574949253</v>
+      </c>
+      <c r="AD101">
+        <v>0.61790187764541005</v>
+      </c>
+    </row>
+    <row r="102" spans="1:30" ht="25.5">
+      <c r="A102" s="12"/>
+      <c r="B102" s="12"/>
+      <c r="C102" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D102">
+        <v>30.091683223095</v>
+      </c>
+      <c r="E102">
+        <v>11.084275392442899</v>
+      </c>
+      <c r="F102">
+        <v>2.3918282688257899</v>
+      </c>
+      <c r="G102">
+        <v>9.3717019732631197</v>
+      </c>
+      <c r="H102">
+        <v>5.77341978621227</v>
+      </c>
+      <c r="I102">
+        <v>5.69028728293498</v>
+      </c>
+      <c r="J102">
+        <v>3.1145384520478401</v>
+      </c>
+      <c r="K102">
+        <v>5.7750464726253101</v>
+      </c>
+      <c r="L102">
+        <v>1.34523148502693</v>
+      </c>
+      <c r="M102">
+        <v>5.5537316138547101</v>
+      </c>
+      <c r="N102">
+        <v>7.4097685390113499</v>
+      </c>
+      <c r="O102">
+        <v>3.2502011686371501</v>
+      </c>
+      <c r="P102">
+        <v>5.2433257979331804</v>
+      </c>
+      <c r="Q102">
+        <v>9.75628461880063E-2</v>
+      </c>
+      <c r="R102">
+        <v>4.2601307128980501</v>
+      </c>
+      <c r="S102">
+        <v>0.18975102383193801</v>
+      </c>
+      <c r="T102">
+        <v>0.40023975371135501</v>
+      </c>
+      <c r="U102">
+        <v>7.9072761460186403</v>
+      </c>
+      <c r="V102">
+        <v>0.729449746736342</v>
+      </c>
+      <c r="W102">
+        <v>6.7797855825676496</v>
+      </c>
+      <c r="X102">
+        <v>7.40446589423268</v>
+      </c>
+      <c r="Y102">
+        <v>8.3209905477313999</v>
+      </c>
+      <c r="Z102">
+        <v>5.4671682987415098</v>
+      </c>
+      <c r="AA102">
+        <v>1.4699680711798999</v>
+      </c>
+      <c r="AB102">
+        <v>0.69597271490619494</v>
+      </c>
+      <c r="AC102">
+        <v>1.0462691201160199</v>
+      </c>
+      <c r="AD102">
+        <v>2.7037169695933998</v>
+      </c>
+    </row>
+    <row r="103" spans="1:30" ht="25.5">
+      <c r="A103" s="12"/>
+      <c r="B103" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D103">
+        <v>30</v>
+      </c>
+      <c r="E103">
+        <v>17.888543819998301</v>
+      </c>
+      <c r="F103">
+        <v>1.4769228991386101</v>
+      </c>
+      <c r="G103">
+        <v>9.8129653083290602</v>
+      </c>
+      <c r="H103">
+        <v>4.3032320157286801</v>
+      </c>
+      <c r="I103">
+        <v>2.8556753840442801</v>
+      </c>
+      <c r="J103">
+        <v>2.2069648374459199</v>
+      </c>
+      <c r="K103">
+        <v>2.7369517151480398</v>
+      </c>
+      <c r="L103">
+        <v>2.1092639734694001</v>
+      </c>
+      <c r="M103">
+        <v>1.1595736856212</v>
+      </c>
+      <c r="N103">
+        <v>2.0312047023012698</v>
+      </c>
+      <c r="O103">
+        <v>4.6983087216154198</v>
+      </c>
+      <c r="P103">
+        <v>10.4661454604472</v>
+      </c>
+      <c r="Q103">
+        <v>2.1473346920106802</v>
+      </c>
+      <c r="R103">
+        <v>2.6766864466929001</v>
+      </c>
+      <c r="S103">
+        <v>1.44471488236921</v>
+      </c>
+      <c r="T103">
+        <v>1.9418158290821801</v>
+      </c>
+      <c r="U103">
+        <v>4.72610991806605</v>
+      </c>
+      <c r="V103">
+        <v>2.0208852585425698</v>
+      </c>
+      <c r="W103">
+        <v>13.9744639851711</v>
+      </c>
+      <c r="X103">
+        <v>5.7282848679727696</v>
+      </c>
+      <c r="Y103">
+        <v>2.3421187289433201</v>
+      </c>
+      <c r="Z103">
+        <v>2.9084194525234599</v>
+      </c>
+      <c r="AA103">
+        <v>3.2197709823663598</v>
+      </c>
+      <c r="AB103">
+        <v>10.908070516518301</v>
+      </c>
+      <c r="AC103">
+        <v>2.1109703716724502</v>
+      </c>
+      <c r="AD103">
+        <v>1.4700682639178699</v>
+      </c>
+    </row>
+    <row r="104" spans="1:30" ht="25.5">
+      <c r="A104" s="12"/>
+      <c r="B104" s="12"/>
+      <c r="C104" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D104">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E104">
+        <v>12.0747670784988</v>
+      </c>
+      <c r="F104">
+        <v>2.41992245564977</v>
+      </c>
+      <c r="G104">
+        <v>0.88906093532768304</v>
+      </c>
+      <c r="H104">
+        <v>20.33250909489</v>
+      </c>
+      <c r="I104">
+        <v>2.09420745774937E-2</v>
+      </c>
+      <c r="J104">
+        <v>1.73602756043779E-2</v>
+      </c>
+      <c r="K104">
+        <v>9.0765422604366902E-2</v>
+      </c>
+      <c r="L104">
+        <v>10.6855477471131</v>
+      </c>
+      <c r="M104">
+        <v>0.10823641371888899</v>
+      </c>
+      <c r="N104">
+        <v>3.7801988126144499</v>
+      </c>
+      <c r="O104">
+        <v>2.7522098111036701</v>
+      </c>
+      <c r="P104">
+        <v>2.0757654407030202E-2</v>
+      </c>
+      <c r="Q104">
+        <v>7.7436204030911296E-2</v>
+      </c>
+      <c r="R104" s="10">
+        <v>4.0778069467589798E-7</v>
+      </c>
+      <c r="S104">
+        <v>4.5623549141792397E-2</v>
+      </c>
+      <c r="T104">
+        <v>0.24245470156520799</v>
+      </c>
+      <c r="U104">
+        <v>25.380418828936399</v>
+      </c>
+      <c r="V104">
+        <v>1.21355385501884E-2</v>
+      </c>
+      <c r="W104">
+        <v>0.11536879938611</v>
+      </c>
+      <c r="X104">
+        <v>20.1226995559012</v>
+      </c>
+      <c r="Y104">
+        <v>2.7475090278152399</v>
+      </c>
+      <c r="Z104">
+        <v>0.40512382780073702</v>
+      </c>
+      <c r="AA104">
+        <v>1.2903940167469501E-4</v>
+      </c>
+      <c r="AB104">
+        <v>10.682639425451001</v>
+      </c>
+      <c r="AC104">
+        <v>0.176177505553097</v>
+      </c>
+      <c r="AD104">
+        <v>1.29469534672436</v>
+      </c>
+    </row>
+    <row r="105" spans="1:30" ht="25.5">
+      <c r="A105" s="12"/>
+      <c r="B105" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D105">
+        <v>28.7326231272157</v>
+      </c>
+      <c r="E105">
+        <v>17.723062492518601</v>
+      </c>
+      <c r="F105">
+        <v>141.920298130378</v>
+      </c>
+      <c r="G105">
+        <v>7.0271525469390603</v>
+      </c>
+      <c r="H105">
+        <v>5.7558254890402196</v>
+      </c>
+      <c r="I105">
+        <v>6.1796011750064999</v>
+      </c>
+      <c r="J105">
+        <v>3.63694705920881</v>
+      </c>
+      <c r="K105">
+        <v>4.9082741171076503</v>
+      </c>
+      <c r="L105">
+        <v>3.2131713732425302</v>
+      </c>
+      <c r="M105">
+        <v>1.0942929434111199</v>
+      </c>
+      <c r="N105">
+        <v>4.0607227451750898</v>
+      </c>
+      <c r="O105">
+        <v>3.63694705920881</v>
+      </c>
+      <c r="P105">
+        <v>3.63694705920881</v>
+      </c>
+      <c r="Q105">
+        <v>4.48449843114137</v>
+      </c>
+      <c r="R105">
+        <v>7.0271525469390603</v>
+      </c>
+      <c r="S105">
+        <v>3.63694705920881</v>
+      </c>
+      <c r="T105">
+        <v>2.3656200013099702</v>
+      </c>
+      <c r="U105">
+        <v>7.0271525469390603</v>
+      </c>
+      <c r="V105">
+        <v>5.7558254890402196</v>
+      </c>
+      <c r="W105">
+        <v>1.94184431534369</v>
+      </c>
+      <c r="X105">
+        <v>5.3320498030739296</v>
+      </c>
+      <c r="Y105">
+        <v>3.63694705920881</v>
+      </c>
+      <c r="Z105">
+        <v>1.0942929434111199</v>
+      </c>
+      <c r="AA105">
+        <v>2.3656200013099702</v>
+      </c>
+      <c r="AB105">
+        <v>5.3320498030739296</v>
+      </c>
+      <c r="AC105">
+        <v>1.5180686293773999</v>
+      </c>
+      <c r="AD105">
+        <v>5.3320498030739296</v>
+      </c>
+    </row>
+    <row r="106" spans="1:30" ht="25.5">
+      <c r="A106" s="12"/>
+      <c r="B106" s="12"/>
+      <c r="C106" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D106">
+        <v>29.587014422325201</v>
+      </c>
+      <c r="E106">
+        <v>11.4611296056797</v>
+      </c>
+      <c r="F106">
+        <v>226.91493174841099</v>
+      </c>
+      <c r="G106">
+        <v>6.50651259160996</v>
+      </c>
+      <c r="H106">
+        <v>6.50651259160996</v>
+      </c>
+      <c r="I106">
+        <v>5.5859174735994799</v>
+      </c>
+      <c r="J106">
+        <v>4.6653223555889998</v>
+      </c>
+      <c r="K106">
+        <v>5.1256199145942398</v>
+      </c>
+      <c r="L106">
+        <v>1.44323944255234</v>
+      </c>
+      <c r="M106">
+        <v>6.50651259160996</v>
+      </c>
+      <c r="N106">
+        <v>1.44323944255234</v>
+      </c>
+      <c r="O106">
+        <v>3.7447272375785299</v>
+      </c>
+      <c r="P106">
+        <v>6.50651259160996</v>
+      </c>
+      <c r="Q106">
+        <v>1.9035370015575701</v>
+      </c>
+      <c r="R106">
+        <v>4.6653223555889998</v>
+      </c>
+      <c r="S106">
+        <v>2.8241321195680502</v>
+      </c>
+      <c r="T106">
+        <v>1.44323944255234</v>
+      </c>
+      <c r="U106">
+        <v>3.7447272375785299</v>
+      </c>
+      <c r="V106">
+        <v>1.9035370015575701</v>
+      </c>
+      <c r="W106">
+        <v>2.8241321195680502</v>
+      </c>
+      <c r="X106">
+        <v>2.3638345605628102</v>
+      </c>
+      <c r="Y106">
+        <v>5.5859174735994799</v>
+      </c>
+      <c r="Z106">
+        <v>2.8241321195680502</v>
+      </c>
+      <c r="AA106">
+        <v>6.50651259160996</v>
+      </c>
+      <c r="AB106">
+        <v>7.8874052686256704</v>
+      </c>
+      <c r="AC106">
+        <v>1.44323944255234</v>
+      </c>
+      <c r="AD106">
+        <v>6.0462150326047199</v>
+      </c>
+    </row>
+    <row r="109" spans="1:30" ht="25.5">
+      <c r="A109" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B109" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D109">
+        <v>29.428662673760801</v>
+      </c>
+      <c r="E109">
+        <v>17.139315168134701</v>
+      </c>
+      <c r="F109">
+        <v>1.50815026272569</v>
+      </c>
+      <c r="G109">
+        <v>7.22152890090097</v>
+      </c>
+      <c r="H109">
+        <v>7.6012345065165103</v>
+      </c>
+      <c r="I109">
+        <v>2.1592382382965498</v>
+      </c>
+      <c r="J109">
+        <v>4.0750520454607102</v>
+      </c>
+      <c r="K109">
+        <v>5.4049511325980797</v>
+      </c>
+      <c r="L109">
+        <v>1.1394118971587099</v>
+      </c>
+      <c r="M109">
+        <v>4.3496615466374999</v>
+      </c>
+      <c r="N109">
+        <v>3.23792232052228</v>
+      </c>
+      <c r="O109">
+        <v>0.53666809160256801</v>
+      </c>
+      <c r="P109">
+        <v>6.92956919071126</v>
+      </c>
+      <c r="Q109">
+        <v>2.19619952250327</v>
+      </c>
+      <c r="R109">
+        <v>7.8705074605868797</v>
+      </c>
+      <c r="S109">
+        <v>0.95859947953693003</v>
+      </c>
+      <c r="T109">
+        <v>0.68666019157685898</v>
+      </c>
+      <c r="U109">
+        <v>7.9521660032603698</v>
+      </c>
+      <c r="V109">
+        <v>5.8624506488922004</v>
+      </c>
+      <c r="W109">
+        <v>5.8730082157919297</v>
+      </c>
+      <c r="X109">
+        <v>4.7943282891268098</v>
+      </c>
+      <c r="Y109">
+        <v>5.6143134777887296</v>
+      </c>
+      <c r="Z109">
+        <v>1.90924489856045</v>
+      </c>
+      <c r="AA109">
+        <v>3.78780630190372</v>
+      </c>
+      <c r="AB109">
+        <v>7.7614400129287002</v>
+      </c>
+      <c r="AC109">
+        <v>1.46013574949253</v>
+      </c>
+      <c r="AD109">
+        <v>0.61790187764541005</v>
+      </c>
+    </row>
+    <row r="110" spans="1:30" ht="25.5">
+      <c r="A110" s="12"/>
+      <c r="B110" s="12"/>
+      <c r="C110" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D110">
+        <v>30.091683223095</v>
+      </c>
+      <c r="E110">
+        <v>11.084275392442899</v>
+      </c>
+      <c r="F110">
+        <v>2.3918282688257899</v>
+      </c>
+      <c r="G110">
+        <v>9.3717019732631197</v>
+      </c>
+      <c r="H110">
+        <v>5.77341978621227</v>
+      </c>
+      <c r="I110">
+        <v>5.69028728293498</v>
+      </c>
+      <c r="J110">
+        <v>3.1145384520478401</v>
+      </c>
+      <c r="K110">
+        <v>5.7750464726253101</v>
+      </c>
+      <c r="L110">
+        <v>1.34523148502693</v>
+      </c>
+      <c r="M110">
+        <v>5.5537316138547101</v>
+      </c>
+      <c r="N110">
+        <v>7.4097685390113499</v>
+      </c>
+      <c r="O110">
+        <v>3.2502011686371501</v>
+      </c>
+      <c r="P110">
+        <v>5.2433257979331804</v>
+      </c>
+      <c r="Q110">
+        <v>9.75628461880063E-2</v>
+      </c>
+      <c r="R110">
+        <v>4.2601307128980501</v>
+      </c>
+      <c r="S110">
+        <v>0.18975102383193801</v>
+      </c>
+      <c r="T110">
+        <v>0.40023975371135501</v>
+      </c>
+      <c r="U110">
+        <v>7.9072761460186403</v>
+      </c>
+      <c r="V110">
+        <v>0.729449746736342</v>
+      </c>
+      <c r="W110">
+        <v>6.7797855825676496</v>
+      </c>
+      <c r="X110">
+        <v>7.40446589423268</v>
+      </c>
+      <c r="Y110">
+        <v>8.3209905477313999</v>
+      </c>
+      <c r="Z110">
+        <v>5.4671682987415098</v>
+      </c>
+      <c r="AA110">
+        <v>1.4699680711798999</v>
+      </c>
+      <c r="AB110">
+        <v>0.69597271490619494</v>
+      </c>
+      <c r="AC110">
+        <v>1.0462691201160199</v>
+      </c>
+      <c r="AD110">
+        <v>2.7037169695933998</v>
+      </c>
+    </row>
+    <row r="111" spans="1:30" ht="25.5">
+      <c r="A111" s="12"/>
+      <c r="B111" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="112" spans="1:30" ht="25.5">
+      <c r="A112" s="12"/>
+      <c r="B112" s="12"/>
+      <c r="C112" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="25.5">
+      <c r="A113" s="12"/>
+      <c r="B113" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="25.5">
+      <c r="A114" s="12"/>
+      <c r="B114" s="12"/>
+      <c r="C114" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="60">
+    <mergeCell ref="A101:A106"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="B105:B106"/>
+    <mergeCell ref="A109:A114"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A46:A51"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A54:A59"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="A70:A75"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B74:B75"/>
     <mergeCell ref="A93:A98"/>
     <mergeCell ref="B93:B94"/>
     <mergeCell ref="B95:B96"/>
@@ -7458,46 +8584,6 @@
     <mergeCell ref="B85:B86"/>
     <mergeCell ref="B87:B88"/>
     <mergeCell ref="B89:B90"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="A70:A75"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="A46:A51"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="A54:A59"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A38:A43"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -7518,111 +8604,111 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="6" customWidth="1"/>
-    <col min="2" max="1024" width="11.5703125" style="6"/>
+    <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
+    <col min="2" max="1024" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="9">
         <v>1.4165359383584</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="1">
         <v>342</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="1">
         <v>0.65687968338236802</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="1">
         <v>0.296208323</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="1">
         <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="5"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="12" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="1">
         <v>2.2667210120000001</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="1">
         <v>490</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="1">
         <v>0.38197667499999999</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="1">
         <v>0.28745091</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="1">
         <v>389</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="8"/>
+      <c r="A8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="1">
         <v>1.4281900000000001</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="1">
         <v>267</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="1">
         <v>0.2057274</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="1">
         <v>0.16775899999999999</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="1">
         <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="5"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="12" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D10">
@@ -7642,31 +8728,31 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="5"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="12" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D15">
@@ -7686,9 +8772,9 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="5"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="12" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D16">
@@ -7708,13 +8794,13 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D18">
@@ -7734,9 +8820,9 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="5"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="12" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D19">
@@ -7756,31 +8842,31 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="5"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="12" t="s">
+      <c r="A22" s="12"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D24">
@@ -7800,9 +8886,9 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="5"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="12" t="s">
+      <c r="A25" s="12"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D25">
@@ -7823,6 +8909,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A15:A16"/>
@@ -7831,12 +8923,6 @@
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -7872,13 +8958,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D4">
@@ -7892,9 +8978,9 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="5"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="12" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
22jan2016 output for MVO
</commit_message>
<xml_diff>
--- a/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
+++ b/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="59">
   <si>
     <t>Date range</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>21-Jan-2016 ::20-Jan-2021</t>
+  </si>
+  <si>
+    <t>22-Jan-2016 ::21-Jan-2021</t>
   </si>
 </sst>
 </file>
@@ -694,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMJ114"/>
+  <dimension ref="A1:AMJ122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110:AD110"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117:C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -8498,6 +8501,87 @@
       <c r="C111" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="D111">
+        <v>33.4</v>
+      </c>
+      <c r="E111">
+        <v>19.677398201998098</v>
+      </c>
+      <c r="F111">
+        <v>1.5154442520237199</v>
+      </c>
+      <c r="G111">
+        <v>0.47987922164708002</v>
+      </c>
+      <c r="H111">
+        <v>18.048527105080399</v>
+      </c>
+      <c r="I111">
+        <v>6.8790684485603396E-2</v>
+      </c>
+      <c r="J111">
+        <v>10.866830747248599</v>
+      </c>
+      <c r="K111">
+        <v>1.4422784516776099</v>
+      </c>
+      <c r="L111">
+        <v>2.9170648321220898</v>
+      </c>
+      <c r="M111">
+        <v>0.49462477373949398</v>
+      </c>
+      <c r="N111">
+        <v>5.6665043979762304</v>
+      </c>
+      <c r="O111">
+        <v>1.8767181167590301</v>
+      </c>
+      <c r="P111">
+        <v>3.52440302001113</v>
+      </c>
+      <c r="Q111">
+        <v>0.94820405400152197</v>
+      </c>
+      <c r="R111">
+        <v>8.8451858653580508</v>
+      </c>
+      <c r="S111">
+        <v>2.7738027362779301</v>
+      </c>
+      <c r="T111">
+        <v>0.19022193383197999</v>
+      </c>
+      <c r="U111">
+        <v>6.4269567580479698</v>
+      </c>
+      <c r="V111">
+        <v>1.6131107794724899</v>
+      </c>
+      <c r="W111">
+        <v>2.2327912340867</v>
+      </c>
+      <c r="X111">
+        <v>5.0853589321272601</v>
+      </c>
+      <c r="Y111">
+        <v>12.3904643452169</v>
+      </c>
+      <c r="Z111">
+        <v>0.408521500234232</v>
+      </c>
+      <c r="AA111">
+        <v>1.3009129234363399</v>
+      </c>
+      <c r="AB111">
+        <v>10.216944173182201</v>
+      </c>
+      <c r="AC111">
+        <v>0.29163151022262501</v>
+      </c>
+      <c r="AD111">
+        <v>1.89027190375638</v>
+      </c>
     </row>
     <row r="112" spans="1:30" ht="25.5">
       <c r="A112" s="12"/>
@@ -8505,6 +8589,87 @@
       <c r="C112" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="D112">
+        <v>29.799999999999901</v>
+      </c>
+      <c r="E112">
+        <v>10.285912696499</v>
+      </c>
+      <c r="F112">
+        <v>2.5491174943497601</v>
+      </c>
+      <c r="G112">
+        <v>2.6894667598878601</v>
+      </c>
+      <c r="H112">
+        <v>1.44825057897888</v>
+      </c>
+      <c r="I112">
+        <v>0.29535931803990301</v>
+      </c>
+      <c r="J112">
+        <v>3.41116246288939</v>
+      </c>
+      <c r="K112">
+        <v>3.1194173485509502</v>
+      </c>
+      <c r="L112">
+        <v>0.70292414011443505</v>
+      </c>
+      <c r="M112">
+        <v>1.1642949845195301</v>
+      </c>
+      <c r="N112">
+        <v>2.3915624182927901</v>
+      </c>
+      <c r="O112">
+        <v>0.45271321248714602</v>
+      </c>
+      <c r="P112">
+        <v>32.521942485900098</v>
+      </c>
+      <c r="Q112">
+        <v>0.94802079957635499</v>
+      </c>
+      <c r="R112">
+        <v>5.4626660436800396</v>
+      </c>
+      <c r="S112">
+        <v>0.41109392157516</v>
+      </c>
+      <c r="T112">
+        <v>0.462314666272921</v>
+      </c>
+      <c r="U112">
+        <v>1.9822502906097501</v>
+      </c>
+      <c r="V112">
+        <v>0.68093908796230895</v>
+      </c>
+      <c r="W112">
+        <v>11.7594048371346</v>
+      </c>
+      <c r="X112">
+        <v>5.8376771926014603</v>
+      </c>
+      <c r="Y112">
+        <v>15.4848990853485</v>
+      </c>
+      <c r="Z112">
+        <v>1.5903086159531199</v>
+      </c>
+      <c r="AA112">
+        <v>1.46092259471825</v>
+      </c>
+      <c r="AB112">
+        <v>2.8952700525155199</v>
+      </c>
+      <c r="AC112">
+        <v>1.3286610545473301</v>
+      </c>
+      <c r="AD112">
+        <v>1.49847804784348</v>
+      </c>
     </row>
     <row r="113" spans="1:3" ht="25.5">
       <c r="A113" s="12"/>
@@ -8522,56 +8687,62 @@
         <v>33</v>
       </c>
     </row>
+    <row r="117" spans="1:3" ht="25.5">
+      <c r="A117" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B117" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="25.5">
+      <c r="A118" s="12"/>
+      <c r="B118" s="12"/>
+      <c r="C118" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="25.5">
+      <c r="A119" s="12"/>
+      <c r="B119" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="25.5">
+      <c r="A120" s="12"/>
+      <c r="B120" s="12"/>
+      <c r="C120" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="25.5">
+      <c r="A121" s="12"/>
+      <c r="B121" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="25.5">
+      <c r="A122" s="12"/>
+      <c r="B122" s="12"/>
+      <c r="C122" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="A101:A106"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="B105:B106"/>
-    <mergeCell ref="A109:A114"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="B113:B114"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A38:A43"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A46:A51"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="A54:A59"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="A70:A75"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B74:B75"/>
+  <mergeCells count="64">
+    <mergeCell ref="A117:A122"/>
+    <mergeCell ref="B117:B118"/>
+    <mergeCell ref="B119:B120"/>
+    <mergeCell ref="B121:B122"/>
     <mergeCell ref="A93:A98"/>
     <mergeCell ref="B93:B94"/>
     <mergeCell ref="B95:B96"/>
@@ -8584,6 +8755,54 @@
     <mergeCell ref="B85:B86"/>
     <mergeCell ref="B87:B88"/>
     <mergeCell ref="B89:B90"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="A70:A75"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="A46:A51"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A54:A59"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A101:A106"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="B105:B106"/>
+    <mergeCell ref="A109:A114"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="B113:B114"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -8909,12 +9128,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A15:A16"/>
@@ -8923,6 +9136,12 @@
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
22jan outputs and edits
</commit_message>
<xml_diff>
--- a/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
+++ b/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
@@ -699,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMJ122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117:C122"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120:AD120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -8671,7 +8671,7 @@
         <v>1.49847804784348</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="25.5">
+    <row r="113" spans="1:30" ht="25.5">
       <c r="A113" s="12"/>
       <c r="B113" s="15" t="s">
         <v>35</v>
@@ -8680,14 +8680,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="25.5">
+    <row r="114" spans="1:30" ht="25.5">
       <c r="A114" s="12"/>
       <c r="B114" s="12"/>
       <c r="C114" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="25.5">
+    <row r="117" spans="1:30" ht="25.5">
       <c r="A117" s="11" t="s">
         <v>58</v>
       </c>
@@ -8697,15 +8697,177 @@
       <c r="C117" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" ht="25.5">
+      <c r="D117">
+        <v>31.459894543635802</v>
+      </c>
+      <c r="E117">
+        <v>18.5937613105846</v>
+      </c>
+      <c r="F117">
+        <v>1.49942198772686</v>
+      </c>
+      <c r="G117">
+        <v>8.3354882886577499</v>
+      </c>
+      <c r="H117">
+        <v>10.168161786263299</v>
+      </c>
+      <c r="I117">
+        <v>3.63141257072634</v>
+      </c>
+      <c r="J117">
+        <v>3.3279260701063702</v>
+      </c>
+      <c r="K117">
+        <v>8.5257875628452098</v>
+      </c>
+      <c r="L117">
+        <v>2.18999681499854</v>
+      </c>
+      <c r="M117">
+        <v>0.66079255642718804</v>
+      </c>
+      <c r="N117">
+        <v>1.7120986144772301</v>
+      </c>
+      <c r="O117">
+        <v>1.04286390106311</v>
+      </c>
+      <c r="P117">
+        <v>1.24604959225402</v>
+      </c>
+      <c r="Q117">
+        <v>0.27036638129784102</v>
+      </c>
+      <c r="R117">
+        <v>1.4629522778995001</v>
+      </c>
+      <c r="S117">
+        <v>9.9485649711311996</v>
+      </c>
+      <c r="T117">
+        <v>0.84205365544404998</v>
+      </c>
+      <c r="U117">
+        <v>10.096078972665699</v>
+      </c>
+      <c r="V117">
+        <v>0.84109573674310401</v>
+      </c>
+      <c r="W117">
+        <v>9.8217621380487508</v>
+      </c>
+      <c r="X117">
+        <v>7.0878702815849701</v>
+      </c>
+      <c r="Y117">
+        <v>1.4627173020584801</v>
+      </c>
+      <c r="Z117">
+        <v>2.2584040824045801</v>
+      </c>
+      <c r="AA117">
+        <v>4.1569504118447798</v>
+      </c>
+      <c r="AB117">
+        <v>6.2380145287178799</v>
+      </c>
+      <c r="AC117">
+        <v>1.48117420540989</v>
+      </c>
+      <c r="AD117">
+        <v>3.1914172969300001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:30" ht="25.5">
       <c r="A118" s="12"/>
       <c r="B118" s="12"/>
       <c r="C118" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" ht="25.5">
+      <c r="D118">
+        <v>31.459894543635802</v>
+      </c>
+      <c r="E118">
+        <v>11.7453225386335</v>
+      </c>
+      <c r="F118">
+        <v>2.3737019100098098</v>
+      </c>
+      <c r="G118">
+        <v>8.3354882886577499</v>
+      </c>
+      <c r="H118">
+        <v>10.168161786263299</v>
+      </c>
+      <c r="I118">
+        <v>3.63141257072634</v>
+      </c>
+      <c r="J118">
+        <v>3.3279260701063702</v>
+      </c>
+      <c r="K118">
+        <v>8.5257875628452098</v>
+      </c>
+      <c r="L118">
+        <v>2.18999681499854</v>
+      </c>
+      <c r="M118">
+        <v>0.66079255642718804</v>
+      </c>
+      <c r="N118">
+        <v>1.7120986144772301</v>
+      </c>
+      <c r="O118">
+        <v>1.04286390106311</v>
+      </c>
+      <c r="P118">
+        <v>1.24604959225402</v>
+      </c>
+      <c r="Q118">
+        <v>0.27036638129784102</v>
+      </c>
+      <c r="R118">
+        <v>1.4629522778995001</v>
+      </c>
+      <c r="S118">
+        <v>9.9485649711311996</v>
+      </c>
+      <c r="T118">
+        <v>0.84205365544404998</v>
+      </c>
+      <c r="U118">
+        <v>10.096078972665699</v>
+      </c>
+      <c r="V118">
+        <v>0.84109573674310401</v>
+      </c>
+      <c r="W118">
+        <v>9.8217621380487508</v>
+      </c>
+      <c r="X118">
+        <v>7.0878702815849701</v>
+      </c>
+      <c r="Y118">
+        <v>1.4627173020584801</v>
+      </c>
+      <c r="Z118">
+        <v>2.2584040824045801</v>
+      </c>
+      <c r="AA118">
+        <v>4.1569504118447798</v>
+      </c>
+      <c r="AB118">
+        <v>6.2380145287178799</v>
+      </c>
+      <c r="AC118">
+        <v>1.48117420540989</v>
+      </c>
+      <c r="AD118">
+        <v>3.1914172969300001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:30" ht="25.5">
       <c r="A119" s="12"/>
       <c r="B119" s="14" t="s">
         <v>34</v>
@@ -8713,15 +8875,177 @@
       <c r="C119" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" ht="25.5">
+      <c r="D119">
+        <v>29.599999999999898</v>
+      </c>
+      <c r="E119">
+        <v>17.441330224498302</v>
+      </c>
+      <c r="F119">
+        <v>1.49185868652678</v>
+      </c>
+      <c r="G119">
+        <v>2.2131735371629699</v>
+      </c>
+      <c r="H119">
+        <v>8.7255794817166201</v>
+      </c>
+      <c r="I119">
+        <v>2.6821622452719298</v>
+      </c>
+      <c r="J119">
+        <v>2.6711571208845202</v>
+      </c>
+      <c r="K119">
+        <v>9.7195304822190796</v>
+      </c>
+      <c r="L119">
+        <v>2.20097046268378</v>
+      </c>
+      <c r="M119">
+        <v>1.0507783338008601</v>
+      </c>
+      <c r="N119">
+        <v>7.4071514913996097</v>
+      </c>
+      <c r="O119">
+        <v>2.1942825153477798</v>
+      </c>
+      <c r="P119">
+        <v>0.68888319023443101</v>
+      </c>
+      <c r="Q119">
+        <v>0.46348610234611498</v>
+      </c>
+      <c r="R119">
+        <v>3.0891642703740199</v>
+      </c>
+      <c r="S119">
+        <v>1.4811759324995899</v>
+      </c>
+      <c r="T119">
+        <v>2.56284891575176</v>
+      </c>
+      <c r="U119">
+        <v>8.6573606366628297</v>
+      </c>
+      <c r="V119">
+        <v>1.40042227030698</v>
+      </c>
+      <c r="W119">
+        <v>0.89499490725331599</v>
+      </c>
+      <c r="X119">
+        <v>23.930102522885502</v>
+      </c>
+      <c r="Y119">
+        <v>6.8745099484647199</v>
+      </c>
+      <c r="Z119">
+        <v>1.81697830331054</v>
+      </c>
+      <c r="AA119">
+        <v>1.00761117840908</v>
+      </c>
+      <c r="AB119">
+        <v>1.7095395146918899</v>
+      </c>
+      <c r="AC119">
+        <v>3.23717818406061</v>
+      </c>
+      <c r="AD119">
+        <v>3.3209584522613</v>
+      </c>
+    </row>
+    <row r="120" spans="1:30" ht="25.5">
       <c r="A120" s="12"/>
       <c r="B120" s="12"/>
       <c r="C120" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" ht="25.5">
+      <c r="D120">
+        <v>27.799999999999901</v>
+      </c>
+      <c r="E120">
+        <v>10.285912696499</v>
+      </c>
+      <c r="F120">
+        <v>2.3546768006541199</v>
+      </c>
+      <c r="G120">
+        <v>1.65028350939709</v>
+      </c>
+      <c r="H120">
+        <v>2.09968751558011</v>
+      </c>
+      <c r="I120">
+        <v>0.90382574626335999</v>
+      </c>
+      <c r="J120">
+        <v>1.06373443281111</v>
+      </c>
+      <c r="K120">
+        <v>15.0806768864361</v>
+      </c>
+      <c r="L120">
+        <v>1.42718498561315</v>
+      </c>
+      <c r="M120">
+        <v>6.7565245602503801</v>
+      </c>
+      <c r="N120">
+        <v>7.8210289279537601</v>
+      </c>
+      <c r="O120">
+        <v>0.235385799737415</v>
+      </c>
+      <c r="P120">
+        <v>0.13344908654881901</v>
+      </c>
+      <c r="Q120">
+        <v>0.66073233234818596</v>
+      </c>
+      <c r="R120">
+        <v>4.5005093083796903E-2</v>
+      </c>
+      <c r="S120">
+        <v>0.28438825605280299</v>
+      </c>
+      <c r="T120">
+        <v>0.63050236986788799</v>
+      </c>
+      <c r="U120">
+        <v>18.0819151193047</v>
+      </c>
+      <c r="V120">
+        <v>1.13043900007137</v>
+      </c>
+      <c r="W120">
+        <v>0.371934486836066</v>
+      </c>
+      <c r="X120">
+        <v>32.721305741341197</v>
+      </c>
+      <c r="Y120">
+        <v>7.5087635519859603E-3</v>
+      </c>
+      <c r="Z120">
+        <v>7.8999426021266403E-3</v>
+      </c>
+      <c r="AA120">
+        <v>2.9055380053674198</v>
+      </c>
+      <c r="AB120">
+        <v>5.6702021231256303</v>
+      </c>
+      <c r="AC120">
+        <v>0.306602093934223</v>
+      </c>
+      <c r="AD120">
+        <v>4.2452219211687597E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:30" ht="25.5">
       <c r="A121" s="12"/>
       <c r="B121" s="15" t="s">
         <v>35</v>
@@ -8730,7 +9054,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="25.5">
+    <row r="122" spans="1:30" ht="25.5">
       <c r="A122" s="12"/>
       <c r="B122" s="12"/>
       <c r="C122" s="7" t="s">
@@ -8739,6 +9063,54 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A46:A51"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A54:A59"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="A70:A75"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="A78:A83"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="A85:A90"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B89:B90"/>
     <mergeCell ref="A117:A122"/>
     <mergeCell ref="B117:B118"/>
     <mergeCell ref="B119:B120"/>
@@ -8747,54 +9119,6 @@
     <mergeCell ref="B93:B94"/>
     <mergeCell ref="B95:B96"/>
     <mergeCell ref="B97:B98"/>
-    <mergeCell ref="A78:A83"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="A85:A90"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="A70:A75"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="A46:A51"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="A54:A59"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A38:A43"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A101:A106"/>
     <mergeCell ref="B101:B102"/>
     <mergeCell ref="B103:B104"/>
@@ -9128,6 +9452,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A15:A16"/>
@@ -9136,12 +9466,6 @@
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
25jan outputs for MVO and PSO
</commit_message>
<xml_diff>
--- a/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
+++ b/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
@@ -317,13 +317,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -332,7 +329,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -699,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMJ122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120:AD120"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="K101" sqref="K101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -804,10 +804,10 @@
       </c>
     </row>
     <row r="2" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -896,8 +896,8 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="25.5">
-      <c r="A3" s="12"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="5" t="s">
         <v>33</v>
       </c>
@@ -984,8 +984,8 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A4" s="12"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -1074,8 +1074,8 @@
       </c>
     </row>
     <row r="5" spans="1:30" ht="25.5">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
@@ -1162,8 +1162,8 @@
       </c>
     </row>
     <row r="6" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1252,8 +1252,8 @@
       </c>
     </row>
     <row r="7" spans="1:30" ht="25.5">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
@@ -1345,10 +1345,10 @@
       <c r="C8"/>
     </row>
     <row r="9" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -1437,8 +1437,8 @@
       </c>
     </row>
     <row r="10" spans="1:30" ht="25.5">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="7" t="s">
         <v>33</v>
       </c>
@@ -1525,8 +1525,8 @@
       </c>
     </row>
     <row r="11" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -1615,8 +1615,8 @@
       </c>
     </row>
     <row r="12" spans="1:30" ht="25.5">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="7" t="s">
         <v>33</v>
       </c>
@@ -1703,8 +1703,8 @@
       </c>
     </row>
     <row r="13" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="15" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -1793,8 +1793,8 @@
       </c>
     </row>
     <row r="14" spans="1:30" ht="25.5">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="7" t="s">
         <v>33</v>
       </c>
@@ -1881,10 +1881,10 @@
       </c>
     </row>
     <row r="16" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -1973,8 +1973,8 @@
       </c>
     </row>
     <row r="17" spans="1:30" ht="25.5">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="7" t="s">
         <v>33</v>
       </c>
@@ -2061,8 +2061,8 @@
       </c>
     </row>
     <row r="18" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A18" s="12"/>
-      <c r="B18" s="14" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -2151,8 +2151,8 @@
       </c>
     </row>
     <row r="19" spans="1:30" ht="25.5">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="7" t="s">
         <v>33</v>
       </c>
@@ -2239,8 +2239,8 @@
       </c>
     </row>
     <row r="20" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A20" s="12"/>
-      <c r="B20" s="15" t="s">
+      <c r="A20" s="11"/>
+      <c r="B20" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -2329,8 +2329,8 @@
       </c>
     </row>
     <row r="21" spans="1:30" ht="25.5">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="7" t="s">
         <v>33</v>
       </c>
@@ -2418,10 +2418,10 @@
     </row>
     <row r="22" spans="1:30" ht="40.5" customHeight="1"/>
     <row r="23" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -2510,8 +2510,8 @@
       </c>
     </row>
     <row r="24" spans="1:30" ht="25.5">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="7" t="s">
         <v>33</v>
       </c>
@@ -2598,8 +2598,8 @@
       </c>
     </row>
     <row r="25" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A25" s="12"/>
-      <c r="B25" s="14" t="s">
+      <c r="A25" s="11"/>
+      <c r="B25" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -2688,8 +2688,8 @@
       </c>
     </row>
     <row r="26" spans="1:30" ht="25.5">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="7" t="s">
         <v>33</v>
       </c>
@@ -2776,8 +2776,8 @@
       </c>
     </row>
     <row r="27" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A27" s="12"/>
-      <c r="B27" s="15" t="s">
+      <c r="A27" s="11"/>
+      <c r="B27" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -2866,8 +2866,8 @@
       </c>
     </row>
     <row r="28" spans="1:30" ht="25.5">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="7" t="s">
         <v>33</v>
       </c>
@@ -2954,10 +2954,10 @@
       </c>
     </row>
     <row r="31" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="6" t="s">
@@ -3046,8 +3046,8 @@
       </c>
     </row>
     <row r="32" spans="1:30" ht="25.5">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="7" t="s">
         <v>33</v>
       </c>
@@ -3134,8 +3134,8 @@
       </c>
     </row>
     <row r="33" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A33" s="12"/>
-      <c r="B33" s="14" t="s">
+      <c r="A33" s="11"/>
+      <c r="B33" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="6" t="s">
@@ -3224,8 +3224,8 @@
       </c>
     </row>
     <row r="34" spans="1:30" ht="25.5">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="7" t="s">
         <v>33</v>
       </c>
@@ -3312,8 +3312,8 @@
       </c>
     </row>
     <row r="35" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A35" s="12"/>
-      <c r="B35" s="15" t="s">
+      <c r="A35" s="11"/>
+      <c r="B35" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -3402,8 +3402,8 @@
       </c>
     </row>
     <row r="36" spans="1:30" ht="25.5">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="7" t="s">
         <v>33</v>
       </c>
@@ -3490,10 +3490,10 @@
       </c>
     </row>
     <row r="38" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="6" t="s">
@@ -3582,8 +3582,8 @@
       </c>
     </row>
     <row r="39" spans="1:30" ht="25.5">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="7" t="s">
         <v>33</v>
       </c>
@@ -3670,8 +3670,8 @@
       </c>
     </row>
     <row r="40" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A40" s="12"/>
-      <c r="B40" s="14" t="s">
+      <c r="A40" s="11"/>
+      <c r="B40" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C40" s="6" t="s">
@@ -3760,8 +3760,8 @@
       </c>
     </row>
     <row r="41" spans="1:30" ht="25.5">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="7" t="s">
         <v>33</v>
       </c>
@@ -3848,8 +3848,8 @@
       </c>
     </row>
     <row r="42" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A42" s="12"/>
-      <c r="B42" s="15" t="s">
+      <c r="A42" s="11"/>
+      <c r="B42" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -3938,8 +3938,8 @@
       </c>
     </row>
     <row r="43" spans="1:30" ht="25.5">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="7" t="s">
         <v>33</v>
       </c>
@@ -4026,10 +4026,10 @@
       </c>
     </row>
     <row r="46" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C46" s="6" t="s">
@@ -4118,8 +4118,8 @@
       </c>
     </row>
     <row r="47" spans="1:30" ht="25.5">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
       <c r="C47" s="7" t="s">
         <v>33</v>
       </c>
@@ -4206,8 +4206,8 @@
       </c>
     </row>
     <row r="48" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A48" s="12"/>
-      <c r="B48" s="14" t="s">
+      <c r="A48" s="11"/>
+      <c r="B48" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -4296,8 +4296,8 @@
       </c>
     </row>
     <row r="49" spans="1:30" ht="25.5">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
       <c r="C49" s="7" t="s">
         <v>33</v>
       </c>
@@ -4384,8 +4384,8 @@
       </c>
     </row>
     <row r="50" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A50" s="12"/>
-      <c r="B50" s="15" t="s">
+      <c r="A50" s="11"/>
+      <c r="B50" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C50" s="6" t="s">
@@ -4474,8 +4474,8 @@
       </c>
     </row>
     <row r="51" spans="1:30" ht="25.5">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
       <c r="C51" s="7" t="s">
         <v>33</v>
       </c>
@@ -4562,10 +4562,10 @@
       </c>
     </row>
     <row r="54" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A54" s="12" t="s">
+      <c r="A54" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C54" s="6" t="s">
@@ -4654,8 +4654,8 @@
       </c>
     </row>
     <row r="55" spans="1:30" ht="25.5">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
+      <c r="A55" s="11"/>
+      <c r="B55" s="11"/>
       <c r="C55" s="7" t="s">
         <v>33</v>
       </c>
@@ -4742,8 +4742,8 @@
       </c>
     </row>
     <row r="56" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A56" s="12"/>
-      <c r="B56" s="14" t="s">
+      <c r="A56" s="11"/>
+      <c r="B56" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C56" s="6" t="s">
@@ -4832,8 +4832,8 @@
       </c>
     </row>
     <row r="57" spans="1:30" ht="25.5">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
       <c r="C57" s="7" t="s">
         <v>33</v>
       </c>
@@ -4920,8 +4920,8 @@
       </c>
     </row>
     <row r="58" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A58" s="12"/>
-      <c r="B58" s="15" t="s">
+      <c r="A58" s="11"/>
+      <c r="B58" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C58" s="6" t="s">
@@ -5010,8 +5010,8 @@
       </c>
     </row>
     <row r="59" spans="1:30" ht="25.5">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12"/>
+      <c r="A59" s="11"/>
+      <c r="B59" s="11"/>
       <c r="C59" s="7" t="s">
         <v>33</v>
       </c>
@@ -5098,10 +5098,10 @@
       </c>
     </row>
     <row r="62" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C62" s="6" t="s">
@@ -5190,8 +5190,8 @@
       </c>
     </row>
     <row r="63" spans="1:30" ht="25.5">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
+      <c r="A63" s="11"/>
+      <c r="B63" s="11"/>
       <c r="C63" s="7" t="s">
         <v>33</v>
       </c>
@@ -5278,8 +5278,8 @@
       </c>
     </row>
     <row r="64" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A64" s="12"/>
-      <c r="B64" s="14" t="s">
+      <c r="A64" s="11"/>
+      <c r="B64" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C64" s="6" t="s">
@@ -5368,8 +5368,8 @@
       </c>
     </row>
     <row r="65" spans="1:30" ht="25.5">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
+      <c r="A65" s="11"/>
+      <c r="B65" s="11"/>
       <c r="C65" s="7" t="s">
         <v>33</v>
       </c>
@@ -5456,8 +5456,8 @@
       </c>
     </row>
     <row r="66" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A66" s="12"/>
-      <c r="B66" s="15" t="s">
+      <c r="A66" s="11"/>
+      <c r="B66" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C66" s="6" t="s">
@@ -5546,8 +5546,8 @@
       </c>
     </row>
     <row r="67" spans="1:30" ht="25.5">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
+      <c r="A67" s="11"/>
+      <c r="B67" s="11"/>
       <c r="C67" s="7" t="s">
         <v>33</v>
       </c>
@@ -5634,10 +5634,10 @@
       </c>
     </row>
     <row r="70" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A70" s="12" t="s">
+      <c r="A70" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C70" s="6" t="s">
@@ -5726,8 +5726,8 @@
       </c>
     </row>
     <row r="71" spans="1:30" ht="25.5">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
+      <c r="A71" s="11"/>
+      <c r="B71" s="11"/>
       <c r="C71" s="7" t="s">
         <v>33</v>
       </c>
@@ -5814,8 +5814,8 @@
       </c>
     </row>
     <row r="72" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A72" s="12"/>
-      <c r="B72" s="14" t="s">
+      <c r="A72" s="11"/>
+      <c r="B72" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C72" s="6" t="s">
@@ -5904,8 +5904,8 @@
       </c>
     </row>
     <row r="73" spans="1:30" ht="25.5">
-      <c r="A73" s="12"/>
-      <c r="B73" s="12"/>
+      <c r="A73" s="11"/>
+      <c r="B73" s="11"/>
       <c r="C73" s="7" t="s">
         <v>33</v>
       </c>
@@ -5992,8 +5992,8 @@
       </c>
     </row>
     <row r="74" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A74" s="12"/>
-      <c r="B74" s="15" t="s">
+      <c r="A74" s="11"/>
+      <c r="B74" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C74" s="6" t="s">
@@ -6082,8 +6082,8 @@
       </c>
     </row>
     <row r="75" spans="1:30" ht="25.5">
-      <c r="A75" s="12"/>
-      <c r="B75" s="12"/>
+      <c r="A75" s="11"/>
+      <c r="B75" s="11"/>
       <c r="C75" s="7" t="s">
         <v>33</v>
       </c>
@@ -6170,10 +6170,10 @@
       </c>
     </row>
     <row r="78" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A78" s="12" t="s">
+      <c r="A78" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B78" s="13" t="s">
+      <c r="B78" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C78" s="6" t="s">
@@ -6262,8 +6262,8 @@
       </c>
     </row>
     <row r="79" spans="1:30" ht="25.5">
-      <c r="A79" s="12"/>
-      <c r="B79" s="12"/>
+      <c r="A79" s="11"/>
+      <c r="B79" s="11"/>
       <c r="C79" s="7" t="s">
         <v>33</v>
       </c>
@@ -6350,8 +6350,8 @@
       </c>
     </row>
     <row r="80" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A80" s="12"/>
-      <c r="B80" s="14" t="s">
+      <c r="A80" s="11"/>
+      <c r="B80" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C80" s="6" t="s">
@@ -6440,8 +6440,8 @@
       </c>
     </row>
     <row r="81" spans="1:30" ht="25.5">
-      <c r="A81" s="12"/>
-      <c r="B81" s="12"/>
+      <c r="A81" s="11"/>
+      <c r="B81" s="11"/>
       <c r="C81" s="7" t="s">
         <v>33</v>
       </c>
@@ -6528,8 +6528,8 @@
       </c>
     </row>
     <row r="82" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A82" s="12"/>
-      <c r="B82" s="15" t="s">
+      <c r="A82" s="11"/>
+      <c r="B82" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C82" s="6" t="s">
@@ -6618,8 +6618,8 @@
       </c>
     </row>
     <row r="83" spans="1:30" ht="25.5">
-      <c r="A83" s="12"/>
-      <c r="B83" s="12"/>
+      <c r="A83" s="11"/>
+      <c r="B83" s="11"/>
       <c r="C83" s="7" t="s">
         <v>33</v>
       </c>
@@ -6706,10 +6706,10 @@
       </c>
     </row>
     <row r="85" spans="1:30" ht="25.5">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B85" s="13" t="s">
+      <c r="B85" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C85" s="6" t="s">
@@ -6798,8 +6798,8 @@
       </c>
     </row>
     <row r="86" spans="1:30" ht="25.5">
-      <c r="A86" s="12"/>
-      <c r="B86" s="12"/>
+      <c r="A86" s="11"/>
+      <c r="B86" s="11"/>
       <c r="C86" s="7" t="s">
         <v>33</v>
       </c>
@@ -6886,8 +6886,8 @@
       </c>
     </row>
     <row r="87" spans="1:30" ht="25.5">
-      <c r="A87" s="12"/>
-      <c r="B87" s="14" t="s">
+      <c r="A87" s="11"/>
+      <c r="B87" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C87" s="6" t="s">
@@ -6976,8 +6976,8 @@
       </c>
     </row>
     <row r="88" spans="1:30" ht="25.5">
-      <c r="A88" s="12"/>
-      <c r="B88" s="12"/>
+      <c r="A88" s="11"/>
+      <c r="B88" s="11"/>
       <c r="C88" s="7" t="s">
         <v>33</v>
       </c>
@@ -7064,8 +7064,8 @@
       </c>
     </row>
     <row r="89" spans="1:30" ht="25.5">
-      <c r="A89" s="12"/>
-      <c r="B89" s="15" t="s">
+      <c r="A89" s="11"/>
+      <c r="B89" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C89" s="6" t="s">
@@ -7154,8 +7154,8 @@
       </c>
     </row>
     <row r="90" spans="1:30" ht="25.5">
-      <c r="A90" s="12"/>
-      <c r="B90" s="12"/>
+      <c r="A90" s="11"/>
+      <c r="B90" s="11"/>
       <c r="C90" s="7" t="s">
         <v>33</v>
       </c>
@@ -7242,10 +7242,10 @@
       </c>
     </row>
     <row r="93" spans="1:30" ht="25.5">
-      <c r="A93" s="11" t="s">
+      <c r="A93" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B93" s="13" t="s">
+      <c r="B93" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C93" s="6" t="s">
@@ -7334,8 +7334,8 @@
       </c>
     </row>
     <row r="94" spans="1:30" ht="25.5">
-      <c r="A94" s="12"/>
-      <c r="B94" s="12"/>
+      <c r="A94" s="11"/>
+      <c r="B94" s="11"/>
       <c r="C94" s="7" t="s">
         <v>33</v>
       </c>
@@ -7422,8 +7422,8 @@
       </c>
     </row>
     <row r="95" spans="1:30" ht="25.5">
-      <c r="A95" s="12"/>
-      <c r="B95" s="14" t="s">
+      <c r="A95" s="11"/>
+      <c r="B95" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C95" s="6" t="s">
@@ -7512,8 +7512,8 @@
       </c>
     </row>
     <row r="96" spans="1:30" ht="25.5">
-      <c r="A96" s="12"/>
-      <c r="B96" s="12"/>
+      <c r="A96" s="11"/>
+      <c r="B96" s="11"/>
       <c r="C96" s="7" t="s">
         <v>33</v>
       </c>
@@ -7600,8 +7600,8 @@
       </c>
     </row>
     <row r="97" spans="1:30" ht="25.5">
-      <c r="A97" s="12"/>
-      <c r="B97" s="15" t="s">
+      <c r="A97" s="11"/>
+      <c r="B97" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C97" s="6" t="s">
@@ -7690,8 +7690,8 @@
       </c>
     </row>
     <row r="98" spans="1:30" ht="25.5">
-      <c r="A98" s="12"/>
-      <c r="B98" s="12"/>
+      <c r="A98" s="11"/>
+      <c r="B98" s="11"/>
       <c r="C98" s="7" t="s">
         <v>33</v>
       </c>
@@ -7702,7 +7702,7 @@
         <v>11.054884989267601</v>
       </c>
       <c r="F98">
-        <v>222.63693645131201</v>
+        <v>2.2263693645131202</v>
       </c>
       <c r="G98">
         <v>6.7990506280679197</v>
@@ -7778,10 +7778,10 @@
       </c>
     </row>
     <row r="101" spans="1:30" ht="25.5">
-      <c r="A101" s="11" t="s">
+      <c r="A101" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B101" s="13" t="s">
+      <c r="B101" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C101" s="6" t="s">
@@ -7870,8 +7870,8 @@
       </c>
     </row>
     <row r="102" spans="1:30" ht="25.5">
-      <c r="A102" s="12"/>
-      <c r="B102" s="12"/>
+      <c r="A102" s="11"/>
+      <c r="B102" s="11"/>
       <c r="C102" s="7" t="s">
         <v>33</v>
       </c>
@@ -7958,8 +7958,8 @@
       </c>
     </row>
     <row r="103" spans="1:30" ht="25.5">
-      <c r="A103" s="12"/>
-      <c r="B103" s="14" t="s">
+      <c r="A103" s="11"/>
+      <c r="B103" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C103" s="6" t="s">
@@ -8048,8 +8048,8 @@
       </c>
     </row>
     <row r="104" spans="1:30" ht="25.5">
-      <c r="A104" s="12"/>
-      <c r="B104" s="12"/>
+      <c r="A104" s="11"/>
+      <c r="B104" s="11"/>
       <c r="C104" s="7" t="s">
         <v>33</v>
       </c>
@@ -8136,8 +8136,8 @@
       </c>
     </row>
     <row r="105" spans="1:30" ht="25.5">
-      <c r="A105" s="12"/>
-      <c r="B105" s="15" t="s">
+      <c r="A105" s="11"/>
+      <c r="B105" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C105" s="6" t="s">
@@ -8226,8 +8226,8 @@
       </c>
     </row>
     <row r="106" spans="1:30" ht="25.5">
-      <c r="A106" s="12"/>
-      <c r="B106" s="12"/>
+      <c r="A106" s="11"/>
+      <c r="B106" s="11"/>
       <c r="C106" s="7" t="s">
         <v>33</v>
       </c>
@@ -8238,7 +8238,7 @@
         <v>11.4611296056797</v>
       </c>
       <c r="F106">
-        <v>226.91493174841099</v>
+        <v>2.2691493174841102</v>
       </c>
       <c r="G106">
         <v>6.50651259160996</v>
@@ -8314,10 +8314,10 @@
       </c>
     </row>
     <row r="109" spans="1:30" ht="25.5">
-      <c r="A109" s="11" t="s">
+      <c r="A109" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B109" s="13" t="s">
+      <c r="B109" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C109" s="6" t="s">
@@ -8406,8 +8406,8 @@
       </c>
     </row>
     <row r="110" spans="1:30" ht="25.5">
-      <c r="A110" s="12"/>
-      <c r="B110" s="12"/>
+      <c r="A110" s="11"/>
+      <c r="B110" s="11"/>
       <c r="C110" s="7" t="s">
         <v>33</v>
       </c>
@@ -8494,8 +8494,8 @@
       </c>
     </row>
     <row r="111" spans="1:30" ht="25.5">
-      <c r="A111" s="12"/>
-      <c r="B111" s="14" t="s">
+      <c r="A111" s="11"/>
+      <c r="B111" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C111" s="6" t="s">
@@ -8584,8 +8584,8 @@
       </c>
     </row>
     <row r="112" spans="1:30" ht="25.5">
-      <c r="A112" s="12"/>
-      <c r="B112" s="12"/>
+      <c r="A112" s="11"/>
+      <c r="B112" s="11"/>
       <c r="C112" s="7" t="s">
         <v>33</v>
       </c>
@@ -8672,8 +8672,8 @@
       </c>
     </row>
     <row r="113" spans="1:30" ht="25.5">
-      <c r="A113" s="12"/>
-      <c r="B113" s="15" t="s">
+      <c r="A113" s="11"/>
+      <c r="B113" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C113" s="6" t="s">
@@ -8681,17 +8681,17 @@
       </c>
     </row>
     <row r="114" spans="1:30" ht="25.5">
-      <c r="A114" s="12"/>
-      <c r="B114" s="12"/>
+      <c r="A114" s="11"/>
+      <c r="B114" s="11"/>
       <c r="C114" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="117" spans="1:30" ht="25.5">
-      <c r="A117" s="11" t="s">
+      <c r="A117" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B117" s="13" t="s">
+      <c r="B117" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C117" s="6" t="s">
@@ -8780,8 +8780,8 @@
       </c>
     </row>
     <row r="118" spans="1:30" ht="25.5">
-      <c r="A118" s="12"/>
-      <c r="B118" s="12"/>
+      <c r="A118" s="11"/>
+      <c r="B118" s="11"/>
       <c r="C118" s="7" t="s">
         <v>33</v>
       </c>
@@ -8868,8 +8868,8 @@
       </c>
     </row>
     <row r="119" spans="1:30" ht="25.5">
-      <c r="A119" s="12"/>
-      <c r="B119" s="14" t="s">
+      <c r="A119" s="11"/>
+      <c r="B119" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C119" s="6" t="s">
@@ -8958,8 +8958,8 @@
       </c>
     </row>
     <row r="120" spans="1:30" ht="25.5">
-      <c r="A120" s="12"/>
-      <c r="B120" s="12"/>
+      <c r="A120" s="11"/>
+      <c r="B120" s="11"/>
       <c r="C120" s="7" t="s">
         <v>33</v>
       </c>
@@ -9046,8 +9046,8 @@
       </c>
     </row>
     <row r="121" spans="1:30" ht="25.5">
-      <c r="A121" s="12"/>
-      <c r="B121" s="15" t="s">
+      <c r="A121" s="11"/>
+      <c r="B121" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C121" s="6" t="s">
@@ -9055,62 +9055,14 @@
       </c>
     </row>
     <row r="122" spans="1:30" ht="25.5">
-      <c r="A122" s="12"/>
-      <c r="B122" s="12"/>
+      <c r="A122" s="11"/>
+      <c r="B122" s="11"/>
       <c r="C122" s="7" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A38:A43"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A46:A51"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="A54:A59"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="A70:A75"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="A78:A83"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="A85:A90"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="B89:B90"/>
     <mergeCell ref="A117:A122"/>
     <mergeCell ref="B117:B118"/>
     <mergeCell ref="B119:B120"/>
@@ -9127,6 +9079,54 @@
     <mergeCell ref="B109:B110"/>
     <mergeCell ref="B111:B112"/>
     <mergeCell ref="B113:B114"/>
+    <mergeCell ref="A78:A83"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="A85:A90"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="A70:A75"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="A46:A51"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A54:A59"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -9172,10 +9172,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -9198,8 +9198,8 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
@@ -9223,10 +9223,10 @@
       <c r="A8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -9249,8 +9249,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="12"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="7" t="s">
         <v>33</v>
       </c>
@@ -9271,10 +9271,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -9282,17 +9282,17 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="12"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -9315,8 +9315,8 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="12"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="7" t="s">
         <v>33</v>
       </c>
@@ -9337,10 +9337,10 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -9363,8 +9363,8 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="12"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="7" t="s">
         <v>33</v>
       </c>
@@ -9385,10 +9385,10 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -9396,17 +9396,17 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="12"/>
-      <c r="B22" s="15"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -9429,8 +9429,8 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="12"/>
-      <c r="B25" s="15"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="7" t="s">
         <v>33</v>
       </c>
@@ -9452,12 +9452,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A15:A16"/>
@@ -9466,6 +9460,12 @@
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -9501,10 +9501,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -9521,8 +9521,8 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="12"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="7" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
27jan MVO and 22jan ACO outputs
</commit_message>
<xml_diff>
--- a/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
+++ b/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="61">
   <si>
     <t>Date range</t>
   </si>
@@ -199,6 +199,12 @@
   <si>
     <t>22-Jan-2016 ::21-Jan-2021</t>
   </si>
+  <si>
+    <t>25-Jan-2016 ::22-Jan-2021</t>
+  </si>
+  <si>
+    <t>27-Jan-2016 ::25-Jan-2021</t>
+  </si>
 </sst>
 </file>
 
@@ -317,10 +323,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -329,10 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -697,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMJ122"/>
+  <dimension ref="A1:AMJ138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="K101" sqref="K101"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="F114" sqref="F114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -804,10 +810,10 @@
       </c>
     </row>
     <row r="2" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -896,8 +902,8 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="25.5">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="5" t="s">
         <v>33</v>
       </c>
@@ -984,8 +990,8 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -1074,8 +1080,8 @@
       </c>
     </row>
     <row r="5" spans="1:30" ht="25.5">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
@@ -1162,8 +1168,8 @@
       </c>
     </row>
     <row r="6" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1252,8 +1258,8 @@
       </c>
     </row>
     <row r="7" spans="1:30" ht="25.5">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
@@ -1345,10 +1351,10 @@
       <c r="C8"/>
     </row>
     <row r="9" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -1437,8 +1443,8 @@
       </c>
     </row>
     <row r="10" spans="1:30" ht="25.5">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="7" t="s">
         <v>33</v>
       </c>
@@ -1525,8 +1531,8 @@
       </c>
     </row>
     <row r="11" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -1615,8 +1621,8 @@
       </c>
     </row>
     <row r="12" spans="1:30" ht="25.5">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="7" t="s">
         <v>33</v>
       </c>
@@ -1703,8 +1709,8 @@
       </c>
     </row>
     <row r="13" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A13" s="11"/>
-      <c r="B13" s="14" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -1793,8 +1799,8 @@
       </c>
     </row>
     <row r="14" spans="1:30" ht="25.5">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="7" t="s">
         <v>33</v>
       </c>
@@ -1881,10 +1887,10 @@
       </c>
     </row>
     <row r="16" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -1973,8 +1979,8 @@
       </c>
     </row>
     <row r="17" spans="1:30" ht="25.5">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="7" t="s">
         <v>33</v>
       </c>
@@ -2061,8 +2067,8 @@
       </c>
     </row>
     <row r="18" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="13" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -2151,8 +2157,8 @@
       </c>
     </row>
     <row r="19" spans="1:30" ht="25.5">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="7" t="s">
         <v>33</v>
       </c>
@@ -2239,8 +2245,8 @@
       </c>
     </row>
     <row r="20" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="14" t="s">
+      <c r="A20" s="12"/>
+      <c r="B20" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -2329,8 +2335,8 @@
       </c>
     </row>
     <row r="21" spans="1:30" ht="25.5">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="7" t="s">
         <v>33</v>
       </c>
@@ -2418,10 +2424,10 @@
     </row>
     <row r="22" spans="1:30" ht="40.5" customHeight="1"/>
     <row r="23" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -2510,8 +2516,8 @@
       </c>
     </row>
     <row r="24" spans="1:30" ht="25.5">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="7" t="s">
         <v>33</v>
       </c>
@@ -2598,8 +2604,8 @@
       </c>
     </row>
     <row r="25" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="13" t="s">
+      <c r="A25" s="12"/>
+      <c r="B25" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -2688,8 +2694,8 @@
       </c>
     </row>
     <row r="26" spans="1:30" ht="25.5">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="7" t="s">
         <v>33</v>
       </c>
@@ -2776,8 +2782,8 @@
       </c>
     </row>
     <row r="27" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="14" t="s">
+      <c r="A27" s="12"/>
+      <c r="B27" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -2866,8 +2872,8 @@
       </c>
     </row>
     <row r="28" spans="1:30" ht="25.5">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="7" t="s">
         <v>33</v>
       </c>
@@ -2954,10 +2960,10 @@
       </c>
     </row>
     <row r="31" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="6" t="s">
@@ -3046,8 +3052,8 @@
       </c>
     </row>
     <row r="32" spans="1:30" ht="25.5">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="7" t="s">
         <v>33</v>
       </c>
@@ -3134,8 +3140,8 @@
       </c>
     </row>
     <row r="33" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A33" s="11"/>
-      <c r="B33" s="13" t="s">
+      <c r="A33" s="12"/>
+      <c r="B33" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="6" t="s">
@@ -3224,8 +3230,8 @@
       </c>
     </row>
     <row r="34" spans="1:30" ht="25.5">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="7" t="s">
         <v>33</v>
       </c>
@@ -3312,8 +3318,8 @@
       </c>
     </row>
     <row r="35" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A35" s="11"/>
-      <c r="B35" s="14" t="s">
+      <c r="A35" s="12"/>
+      <c r="B35" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -3402,8 +3408,8 @@
       </c>
     </row>
     <row r="36" spans="1:30" ht="25.5">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="7" t="s">
         <v>33</v>
       </c>
@@ -3490,10 +3496,10 @@
       </c>
     </row>
     <row r="38" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="6" t="s">
@@ -3582,8 +3588,8 @@
       </c>
     </row>
     <row r="39" spans="1:30" ht="25.5">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="7" t="s">
         <v>33</v>
       </c>
@@ -3670,8 +3676,8 @@
       </c>
     </row>
     <row r="40" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A40" s="11"/>
-      <c r="B40" s="13" t="s">
+      <c r="A40" s="12"/>
+      <c r="B40" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C40" s="6" t="s">
@@ -3760,8 +3766,8 @@
       </c>
     </row>
     <row r="41" spans="1:30" ht="25.5">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
       <c r="C41" s="7" t="s">
         <v>33</v>
       </c>
@@ -3848,8 +3854,8 @@
       </c>
     </row>
     <row r="42" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A42" s="11"/>
-      <c r="B42" s="14" t="s">
+      <c r="A42" s="12"/>
+      <c r="B42" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -3938,8 +3944,8 @@
       </c>
     </row>
     <row r="43" spans="1:30" ht="25.5">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
       <c r="C43" s="7" t="s">
         <v>33</v>
       </c>
@@ -4026,10 +4032,10 @@
       </c>
     </row>
     <row r="46" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C46" s="6" t="s">
@@ -4118,8 +4124,8 @@
       </c>
     </row>
     <row r="47" spans="1:30" ht="25.5">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
       <c r="C47" s="7" t="s">
         <v>33</v>
       </c>
@@ -4206,8 +4212,8 @@
       </c>
     </row>
     <row r="48" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A48" s="11"/>
-      <c r="B48" s="13" t="s">
+      <c r="A48" s="12"/>
+      <c r="B48" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -4296,8 +4302,8 @@
       </c>
     </row>
     <row r="49" spans="1:30" ht="25.5">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
       <c r="C49" s="7" t="s">
         <v>33</v>
       </c>
@@ -4384,8 +4390,8 @@
       </c>
     </row>
     <row r="50" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A50" s="11"/>
-      <c r="B50" s="14" t="s">
+      <c r="A50" s="12"/>
+      <c r="B50" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C50" s="6" t="s">
@@ -4474,8 +4480,8 @@
       </c>
     </row>
     <row r="51" spans="1:30" ht="25.5">
-      <c r="A51" s="11"/>
-      <c r="B51" s="11"/>
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
       <c r="C51" s="7" t="s">
         <v>33</v>
       </c>
@@ -4562,10 +4568,10 @@
       </c>
     </row>
     <row r="54" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C54" s="6" t="s">
@@ -4654,8 +4660,8 @@
       </c>
     </row>
     <row r="55" spans="1:30" ht="25.5">
-      <c r="A55" s="11"/>
-      <c r="B55" s="11"/>
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
       <c r="C55" s="7" t="s">
         <v>33</v>
       </c>
@@ -4742,8 +4748,8 @@
       </c>
     </row>
     <row r="56" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A56" s="11"/>
-      <c r="B56" s="13" t="s">
+      <c r="A56" s="12"/>
+      <c r="B56" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C56" s="6" t="s">
@@ -4832,8 +4838,8 @@
       </c>
     </row>
     <row r="57" spans="1:30" ht="25.5">
-      <c r="A57" s="11"/>
-      <c r="B57" s="11"/>
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
       <c r="C57" s="7" t="s">
         <v>33</v>
       </c>
@@ -4920,8 +4926,8 @@
       </c>
     </row>
     <row r="58" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A58" s="11"/>
-      <c r="B58" s="14" t="s">
+      <c r="A58" s="12"/>
+      <c r="B58" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C58" s="6" t="s">
@@ -5010,8 +5016,8 @@
       </c>
     </row>
     <row r="59" spans="1:30" ht="25.5">
-      <c r="A59" s="11"/>
-      <c r="B59" s="11"/>
+      <c r="A59" s="12"/>
+      <c r="B59" s="12"/>
       <c r="C59" s="7" t="s">
         <v>33</v>
       </c>
@@ -5098,10 +5104,10 @@
       </c>
     </row>
     <row r="62" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C62" s="6" t="s">
@@ -5190,8 +5196,8 @@
       </c>
     </row>
     <row r="63" spans="1:30" ht="25.5">
-      <c r="A63" s="11"/>
-      <c r="B63" s="11"/>
+      <c r="A63" s="12"/>
+      <c r="B63" s="12"/>
       <c r="C63" s="7" t="s">
         <v>33</v>
       </c>
@@ -5278,8 +5284,8 @@
       </c>
     </row>
     <row r="64" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A64" s="11"/>
-      <c r="B64" s="13" t="s">
+      <c r="A64" s="12"/>
+      <c r="B64" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C64" s="6" t="s">
@@ -5368,8 +5374,8 @@
       </c>
     </row>
     <row r="65" spans="1:30" ht="25.5">
-      <c r="A65" s="11"/>
-      <c r="B65" s="11"/>
+      <c r="A65" s="12"/>
+      <c r="B65" s="12"/>
       <c r="C65" s="7" t="s">
         <v>33</v>
       </c>
@@ -5456,8 +5462,8 @@
       </c>
     </row>
     <row r="66" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A66" s="11"/>
-      <c r="B66" s="14" t="s">
+      <c r="A66" s="12"/>
+      <c r="B66" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C66" s="6" t="s">
@@ -5546,8 +5552,8 @@
       </c>
     </row>
     <row r="67" spans="1:30" ht="25.5">
-      <c r="A67" s="11"/>
-      <c r="B67" s="11"/>
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
       <c r="C67" s="7" t="s">
         <v>33</v>
       </c>
@@ -5634,10 +5640,10 @@
       </c>
     </row>
     <row r="70" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A70" s="11" t="s">
+      <c r="A70" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B70" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C70" s="6" t="s">
@@ -5726,8 +5732,8 @@
       </c>
     </row>
     <row r="71" spans="1:30" ht="25.5">
-      <c r="A71" s="11"/>
-      <c r="B71" s="11"/>
+      <c r="A71" s="12"/>
+      <c r="B71" s="12"/>
       <c r="C71" s="7" t="s">
         <v>33</v>
       </c>
@@ -5814,8 +5820,8 @@
       </c>
     </row>
     <row r="72" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A72" s="11"/>
-      <c r="B72" s="13" t="s">
+      <c r="A72" s="12"/>
+      <c r="B72" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C72" s="6" t="s">
@@ -5904,8 +5910,8 @@
       </c>
     </row>
     <row r="73" spans="1:30" ht="25.5">
-      <c r="A73" s="11"/>
-      <c r="B73" s="11"/>
+      <c r="A73" s="12"/>
+      <c r="B73" s="12"/>
       <c r="C73" s="7" t="s">
         <v>33</v>
       </c>
@@ -5992,8 +5998,8 @@
       </c>
     </row>
     <row r="74" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A74" s="11"/>
-      <c r="B74" s="14" t="s">
+      <c r="A74" s="12"/>
+      <c r="B74" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C74" s="6" t="s">
@@ -6082,8 +6088,8 @@
       </c>
     </row>
     <row r="75" spans="1:30" ht="25.5">
-      <c r="A75" s="11"/>
-      <c r="B75" s="11"/>
+      <c r="A75" s="12"/>
+      <c r="B75" s="12"/>
       <c r="C75" s="7" t="s">
         <v>33</v>
       </c>
@@ -6170,10 +6176,10 @@
       </c>
     </row>
     <row r="78" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A78" s="11" t="s">
+      <c r="A78" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B78" s="15" t="s">
+      <c r="B78" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C78" s="6" t="s">
@@ -6262,8 +6268,8 @@
       </c>
     </row>
     <row r="79" spans="1:30" ht="25.5">
-      <c r="A79" s="11"/>
-      <c r="B79" s="11"/>
+      <c r="A79" s="12"/>
+      <c r="B79" s="12"/>
       <c r="C79" s="7" t="s">
         <v>33</v>
       </c>
@@ -6350,8 +6356,8 @@
       </c>
     </row>
     <row r="80" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A80" s="11"/>
-      <c r="B80" s="13" t="s">
+      <c r="A80" s="12"/>
+      <c r="B80" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C80" s="6" t="s">
@@ -6440,8 +6446,8 @@
       </c>
     </row>
     <row r="81" spans="1:30" ht="25.5">
-      <c r="A81" s="11"/>
-      <c r="B81" s="11"/>
+      <c r="A81" s="12"/>
+      <c r="B81" s="12"/>
       <c r="C81" s="7" t="s">
         <v>33</v>
       </c>
@@ -6528,8 +6534,8 @@
       </c>
     </row>
     <row r="82" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A82" s="11"/>
-      <c r="B82" s="14" t="s">
+      <c r="A82" s="12"/>
+      <c r="B82" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C82" s="6" t="s">
@@ -6618,8 +6624,8 @@
       </c>
     </row>
     <row r="83" spans="1:30" ht="25.5">
-      <c r="A83" s="11"/>
-      <c r="B83" s="11"/>
+      <c r="A83" s="12"/>
+      <c r="B83" s="12"/>
       <c r="C83" s="7" t="s">
         <v>33</v>
       </c>
@@ -6706,10 +6712,10 @@
       </c>
     </row>
     <row r="85" spans="1:30" ht="25.5">
-      <c r="A85" s="16" t="s">
+      <c r="A85" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B85" s="15" t="s">
+      <c r="B85" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C85" s="6" t="s">
@@ -6798,8 +6804,8 @@
       </c>
     </row>
     <row r="86" spans="1:30" ht="25.5">
-      <c r="A86" s="11"/>
-      <c r="B86" s="11"/>
+      <c r="A86" s="12"/>
+      <c r="B86" s="12"/>
       <c r="C86" s="7" t="s">
         <v>33</v>
       </c>
@@ -6886,8 +6892,8 @@
       </c>
     </row>
     <row r="87" spans="1:30" ht="25.5">
-      <c r="A87" s="11"/>
-      <c r="B87" s="13" t="s">
+      <c r="A87" s="12"/>
+      <c r="B87" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C87" s="6" t="s">
@@ -6976,8 +6982,8 @@
       </c>
     </row>
     <row r="88" spans="1:30" ht="25.5">
-      <c r="A88" s="11"/>
-      <c r="B88" s="11"/>
+      <c r="A88" s="12"/>
+      <c r="B88" s="12"/>
       <c r="C88" s="7" t="s">
         <v>33</v>
       </c>
@@ -7064,8 +7070,8 @@
       </c>
     </row>
     <row r="89" spans="1:30" ht="25.5">
-      <c r="A89" s="11"/>
-      <c r="B89" s="14" t="s">
+      <c r="A89" s="12"/>
+      <c r="B89" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C89" s="6" t="s">
@@ -7154,8 +7160,8 @@
       </c>
     </row>
     <row r="90" spans="1:30" ht="25.5">
-      <c r="A90" s="11"/>
-      <c r="B90" s="11"/>
+      <c r="A90" s="12"/>
+      <c r="B90" s="12"/>
       <c r="C90" s="7" t="s">
         <v>33</v>
       </c>
@@ -7242,10 +7248,10 @@
       </c>
     </row>
     <row r="93" spans="1:30" ht="25.5">
-      <c r="A93" s="16" t="s">
+      <c r="A93" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="B93" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C93" s="6" t="s">
@@ -7334,8 +7340,8 @@
       </c>
     </row>
     <row r="94" spans="1:30" ht="25.5">
-      <c r="A94" s="11"/>
-      <c r="B94" s="11"/>
+      <c r="A94" s="12"/>
+      <c r="B94" s="12"/>
       <c r="C94" s="7" t="s">
         <v>33</v>
       </c>
@@ -7422,8 +7428,8 @@
       </c>
     </row>
     <row r="95" spans="1:30" ht="25.5">
-      <c r="A95" s="11"/>
-      <c r="B95" s="13" t="s">
+      <c r="A95" s="12"/>
+      <c r="B95" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C95" s="6" t="s">
@@ -7512,8 +7518,8 @@
       </c>
     </row>
     <row r="96" spans="1:30" ht="25.5">
-      <c r="A96" s="11"/>
-      <c r="B96" s="11"/>
+      <c r="A96" s="12"/>
+      <c r="B96" s="12"/>
       <c r="C96" s="7" t="s">
         <v>33</v>
       </c>
@@ -7600,8 +7606,8 @@
       </c>
     </row>
     <row r="97" spans="1:30" ht="25.5">
-      <c r="A97" s="11"/>
-      <c r="B97" s="14" t="s">
+      <c r="A97" s="12"/>
+      <c r="B97" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C97" s="6" t="s">
@@ -7690,8 +7696,8 @@
       </c>
     </row>
     <row r="98" spans="1:30" ht="25.5">
-      <c r="A98" s="11"/>
-      <c r="B98" s="11"/>
+      <c r="A98" s="12"/>
+      <c r="B98" s="12"/>
       <c r="C98" s="7" t="s">
         <v>33</v>
       </c>
@@ -7778,10 +7784,10 @@
       </c>
     </row>
     <row r="101" spans="1:30" ht="25.5">
-      <c r="A101" s="16" t="s">
+      <c r="A101" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B101" s="15" t="s">
+      <c r="B101" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C101" s="6" t="s">
@@ -7870,8 +7876,8 @@
       </c>
     </row>
     <row r="102" spans="1:30" ht="25.5">
-      <c r="A102" s="11"/>
-      <c r="B102" s="11"/>
+      <c r="A102" s="12"/>
+      <c r="B102" s="12"/>
       <c r="C102" s="7" t="s">
         <v>33</v>
       </c>
@@ -7958,8 +7964,8 @@
       </c>
     </row>
     <row r="103" spans="1:30" ht="25.5">
-      <c r="A103" s="11"/>
-      <c r="B103" s="13" t="s">
+      <c r="A103" s="12"/>
+      <c r="B103" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C103" s="6" t="s">
@@ -8048,8 +8054,8 @@
       </c>
     </row>
     <row r="104" spans="1:30" ht="25.5">
-      <c r="A104" s="11"/>
-      <c r="B104" s="11"/>
+      <c r="A104" s="12"/>
+      <c r="B104" s="12"/>
       <c r="C104" s="7" t="s">
         <v>33</v>
       </c>
@@ -8136,8 +8142,8 @@
       </c>
     </row>
     <row r="105" spans="1:30" ht="25.5">
-      <c r="A105" s="11"/>
-      <c r="B105" s="14" t="s">
+      <c r="A105" s="12"/>
+      <c r="B105" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C105" s="6" t="s">
@@ -8226,8 +8232,8 @@
       </c>
     </row>
     <row r="106" spans="1:30" ht="25.5">
-      <c r="A106" s="11"/>
-      <c r="B106" s="11"/>
+      <c r="A106" s="12"/>
+      <c r="B106" s="12"/>
       <c r="C106" s="7" t="s">
         <v>33</v>
       </c>
@@ -8314,10 +8320,10 @@
       </c>
     </row>
     <row r="109" spans="1:30" ht="25.5">
-      <c r="A109" s="16" t="s">
+      <c r="A109" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B109" s="15" t="s">
+      <c r="B109" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C109" s="6" t="s">
@@ -8406,8 +8412,8 @@
       </c>
     </row>
     <row r="110" spans="1:30" ht="25.5">
-      <c r="A110" s="11"/>
-      <c r="B110" s="11"/>
+      <c r="A110" s="12"/>
+      <c r="B110" s="12"/>
       <c r="C110" s="7" t="s">
         <v>33</v>
       </c>
@@ -8494,8 +8500,8 @@
       </c>
     </row>
     <row r="111" spans="1:30" ht="25.5">
-      <c r="A111" s="11"/>
-      <c r="B111" s="13" t="s">
+      <c r="A111" s="12"/>
+      <c r="B111" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C111" s="6" t="s">
@@ -8584,8 +8590,8 @@
       </c>
     </row>
     <row r="112" spans="1:30" ht="25.5">
-      <c r="A112" s="11"/>
-      <c r="B112" s="11"/>
+      <c r="A112" s="12"/>
+      <c r="B112" s="12"/>
       <c r="C112" s="7" t="s">
         <v>33</v>
       </c>
@@ -8672,26 +8678,188 @@
       </c>
     </row>
     <row r="113" spans="1:30" ht="25.5">
-      <c r="A113" s="11"/>
-      <c r="B113" s="14" t="s">
+      <c r="A113" s="12"/>
+      <c r="B113" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="D113">
+        <v>29.907247974865101</v>
+      </c>
+      <c r="E113">
+        <v>17.851405609659199</v>
+      </c>
+      <c r="F113">
+        <v>147.47997188871099</v>
+      </c>
+      <c r="G113">
+        <v>9.6342014684818</v>
+      </c>
+      <c r="H113">
+        <v>9.6342014684818</v>
+      </c>
+      <c r="I113">
+        <v>2.2320005060243799</v>
+      </c>
+      <c r="J113">
+        <v>2.2320005060243799</v>
+      </c>
+      <c r="K113">
+        <v>8.2883467480349999</v>
+      </c>
+      <c r="L113">
+        <v>0.88614578557757995</v>
+      </c>
+      <c r="M113">
+        <v>2.2320005060243799</v>
+      </c>
+      <c r="N113">
+        <v>8.9612741082584009</v>
+      </c>
+      <c r="O113">
+        <v>0.88614578557757995</v>
+      </c>
+      <c r="P113">
+        <v>6.26956466736479</v>
+      </c>
+      <c r="Q113">
+        <v>3.57785522647118</v>
+      </c>
+      <c r="R113">
+        <v>0.88614578557757995</v>
+      </c>
+      <c r="S113">
+        <v>2.2320005060243799</v>
+      </c>
+      <c r="T113">
+        <v>1.5590731458009801</v>
+      </c>
+      <c r="U113">
+        <v>4.2507825866945899</v>
+      </c>
+      <c r="V113">
+        <v>4.9237099469179899</v>
+      </c>
+      <c r="W113">
+        <v>4.2507825866945899</v>
+      </c>
+      <c r="X113">
+        <v>2.2320005060243799</v>
+      </c>
+      <c r="Y113">
+        <v>1.5590731458009801</v>
+      </c>
+      <c r="Z113">
+        <v>1.5590731458009801</v>
+      </c>
+      <c r="AA113">
+        <v>6.9424920275881998</v>
+      </c>
+      <c r="AB113">
+        <v>10.307128828705199</v>
+      </c>
+      <c r="AC113">
+        <v>1.5590731458009801</v>
+      </c>
+      <c r="AD113">
+        <v>2.90492786624778</v>
+      </c>
     </row>
     <row r="114" spans="1:30" ht="25.5">
-      <c r="A114" s="11"/>
-      <c r="B114" s="11"/>
+      <c r="A114" s="12"/>
+      <c r="B114" s="12"/>
       <c r="C114" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="D114">
+        <v>30.169459280157401</v>
+      </c>
+      <c r="E114">
+        <v>11.479328946522701</v>
+      </c>
+      <c r="F114">
+        <v>2.3162903863132001</v>
+      </c>
+      <c r="G114">
+        <v>6.6746228039002498</v>
+      </c>
+      <c r="H114">
+        <v>6.1730315764535302</v>
+      </c>
+      <c r="I114">
+        <v>2.66189298432651</v>
+      </c>
+      <c r="J114">
+        <v>6.1730315764535302</v>
+      </c>
+      <c r="K114">
+        <v>2.66189298432651</v>
+      </c>
+      <c r="L114">
+        <v>1.1571193019863599</v>
+      </c>
+      <c r="M114">
+        <v>4.1666666666666599</v>
+      </c>
+      <c r="N114">
+        <v>1.1571193019863599</v>
+      </c>
+      <c r="O114">
+        <v>3.6650754392199398</v>
+      </c>
+      <c r="P114">
+        <v>6.6746228039002498</v>
+      </c>
+      <c r="Q114">
+        <v>2.16030175687979</v>
+      </c>
+      <c r="R114">
+        <v>5.1698491215600999</v>
+      </c>
+      <c r="S114">
+        <v>6.1730315764535302</v>
+      </c>
+      <c r="T114">
+        <v>1.65871052943307</v>
+      </c>
+      <c r="U114">
+        <v>6.1730315764535302</v>
+      </c>
+      <c r="V114">
+        <v>2.66189298432651</v>
+      </c>
+      <c r="W114">
+        <v>6.1730315764535302</v>
+      </c>
+      <c r="X114">
+        <v>2.66189298432651</v>
+      </c>
+      <c r="Y114">
+        <v>7.1762140313469702</v>
+      </c>
+      <c r="Z114">
+        <v>2.16030175687979</v>
+      </c>
+      <c r="AA114">
+        <v>3.6650754392199398</v>
+      </c>
+      <c r="AB114">
+        <v>7.1762140313469702</v>
+      </c>
+      <c r="AC114">
+        <v>3.6650754392199398</v>
+      </c>
+      <c r="AD114">
+        <v>2.16030175687979</v>
+      </c>
     </row>
     <row r="117" spans="1:30" ht="25.5">
-      <c r="A117" s="16" t="s">
+      <c r="A117" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B117" s="15" t="s">
+      <c r="B117" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C117" s="6" t="s">
@@ -8780,8 +8948,8 @@
       </c>
     </row>
     <row r="118" spans="1:30" ht="25.5">
-      <c r="A118" s="11"/>
-      <c r="B118" s="11"/>
+      <c r="A118" s="12"/>
+      <c r="B118" s="12"/>
       <c r="C118" s="7" t="s">
         <v>33</v>
       </c>
@@ -8868,8 +9036,8 @@
       </c>
     </row>
     <row r="119" spans="1:30" ht="25.5">
-      <c r="A119" s="11"/>
-      <c r="B119" s="13" t="s">
+      <c r="A119" s="12"/>
+      <c r="B119" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C119" s="6" t="s">
@@ -8958,8 +9126,8 @@
       </c>
     </row>
     <row r="120" spans="1:30" ht="25.5">
-      <c r="A120" s="11"/>
-      <c r="B120" s="11"/>
+      <c r="A120" s="12"/>
+      <c r="B120" s="12"/>
       <c r="C120" s="7" t="s">
         <v>33</v>
       </c>
@@ -9046,8 +9214,8 @@
       </c>
     </row>
     <row r="121" spans="1:30" ht="25.5">
-      <c r="A121" s="11"/>
-      <c r="B121" s="14" t="s">
+      <c r="A121" s="12"/>
+      <c r="B121" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C121" s="6" t="s">
@@ -9055,14 +9223,600 @@
       </c>
     </row>
     <row r="122" spans="1:30" ht="25.5">
-      <c r="A122" s="11"/>
-      <c r="B122" s="11"/>
+      <c r="A122" s="12"/>
+      <c r="B122" s="12"/>
       <c r="C122" s="7" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="125" spans="1:30" ht="25.5">
+      <c r="A125" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B125" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D125">
+        <v>29.845396793893102</v>
+      </c>
+      <c r="E125">
+        <v>17.8352618662589</v>
+      </c>
+      <c r="F125">
+        <v>1.4726667312680399</v>
+      </c>
+      <c r="G125">
+        <v>0.38451016277466099</v>
+      </c>
+      <c r="H125">
+        <v>3.4043650844992199</v>
+      </c>
+      <c r="I125">
+        <v>7.9018884909006397</v>
+      </c>
+      <c r="J125">
+        <v>3.10037202916818</v>
+      </c>
+      <c r="K125">
+        <v>8.1028894239994393</v>
+      </c>
+      <c r="L125">
+        <v>1.77370684006032</v>
+      </c>
+      <c r="M125">
+        <v>5.7308257188511398</v>
+      </c>
+      <c r="N125">
+        <v>0.466553189166309</v>
+      </c>
+      <c r="O125">
+        <v>0.53752272463620698</v>
+      </c>
+      <c r="P125">
+        <v>5.4519875415384798</v>
+      </c>
+      <c r="Q125">
+        <v>0.71998149140231604</v>
+      </c>
+      <c r="R125">
+        <v>4.1937722093106302</v>
+      </c>
+      <c r="S125">
+        <v>9.0341514255825395</v>
+      </c>
+      <c r="T125">
+        <v>0.97794634406396996</v>
+      </c>
+      <c r="U125">
+        <v>8.5628421131436898</v>
+      </c>
+      <c r="V125">
+        <v>5.8370332804731104</v>
+      </c>
+      <c r="W125">
+        <v>6.1925038791382603</v>
+      </c>
+      <c r="X125">
+        <v>8.7667321482151692</v>
+      </c>
+      <c r="Y125">
+        <v>7.9595453330024801</v>
+      </c>
+      <c r="Z125">
+        <v>0.59345612880644305</v>
+      </c>
+      <c r="AA125">
+        <v>0.63641870814439006</v>
+      </c>
+      <c r="AB125">
+        <v>7.5284485838682302</v>
+      </c>
+      <c r="AC125">
+        <v>1.49804974001071</v>
+      </c>
+      <c r="AD125">
+        <v>0.64449740924338195</v>
+      </c>
+    </row>
+    <row r="126" spans="1:30" ht="25.5">
+      <c r="A126" s="12"/>
+      <c r="B126" s="12"/>
+      <c r="C126" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D126">
+        <v>28.3016953281405</v>
+      </c>
+      <c r="E126">
+        <v>10.5024848968747</v>
+      </c>
+      <c r="F126">
+        <v>2.3538901099012199</v>
+      </c>
+      <c r="G126">
+        <v>2.0695353329286501</v>
+      </c>
+      <c r="H126">
+        <v>5.2558979716077499</v>
+      </c>
+      <c r="I126">
+        <v>1.2447079566343799</v>
+      </c>
+      <c r="J126">
+        <v>4.3382396367990896</v>
+      </c>
+      <c r="K126">
+        <v>7.8592396681394998</v>
+      </c>
+      <c r="L126">
+        <v>1.1788816222349301</v>
+      </c>
+      <c r="M126">
+        <v>7.7273278985883698</v>
+      </c>
+      <c r="N126">
+        <v>3.7641275113683301</v>
+      </c>
+      <c r="O126">
+        <v>8.1463376971792206E-2</v>
+      </c>
+      <c r="P126">
+        <v>6.5467585169496498</v>
+      </c>
+      <c r="Q126">
+        <v>0.159984518273527</v>
+      </c>
+      <c r="R126">
+        <v>6.5906730703365497</v>
+      </c>
+      <c r="S126">
+        <v>2.4678151260794801</v>
+      </c>
+      <c r="T126">
+        <v>2.96178448360723</v>
+      </c>
+      <c r="U126">
+        <v>7.0285998378968904</v>
+      </c>
+      <c r="V126">
+        <v>2.3249820307998901</v>
+      </c>
+      <c r="W126">
+        <v>7.1040033501593802</v>
+      </c>
+      <c r="X126">
+        <v>6.0012145002905601</v>
+      </c>
+      <c r="Y126">
+        <v>4.6715294335021396</v>
+      </c>
+      <c r="Z126">
+        <v>6.2459363532724899</v>
+      </c>
+      <c r="AA126">
+        <v>0.27738134483930199</v>
+      </c>
+      <c r="AB126">
+        <v>5.3543843337422796</v>
+      </c>
+      <c r="AC126">
+        <v>1.0680658409817501</v>
+      </c>
+      <c r="AD126">
+        <v>7.67746628399596</v>
+      </c>
+    </row>
+    <row r="127" spans="1:30" ht="25.5">
+      <c r="A127" s="12"/>
+      <c r="B127" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D127">
+        <v>27.4</v>
+      </c>
+      <c r="E127">
+        <v>16.546903033498399</v>
+      </c>
+      <c r="F127">
+        <v>1.4395443033525599</v>
+      </c>
+      <c r="G127">
+        <v>5.1688907577179704</v>
+      </c>
+      <c r="H127">
+        <v>0.31000384788876501</v>
+      </c>
+      <c r="I127">
+        <v>5.8442578914507903</v>
+      </c>
+      <c r="J127">
+        <v>0.27067028312646502</v>
+      </c>
+      <c r="K127">
+        <v>4.8817197149098996</v>
+      </c>
+      <c r="L127">
+        <v>4.3534199257070796</v>
+      </c>
+      <c r="M127">
+        <v>0.21968582829692801</v>
+      </c>
+      <c r="N127">
+        <v>10.9554713429676</v>
+      </c>
+      <c r="O127">
+        <v>0.93896982618756197</v>
+      </c>
+      <c r="P127">
+        <v>0.112509871654195</v>
+      </c>
+      <c r="Q127">
+        <v>0.28531439534196801</v>
+      </c>
+      <c r="R127">
+        <v>9.5726074116834301</v>
+      </c>
+      <c r="S127">
+        <v>0.78606763260205104</v>
+      </c>
+      <c r="T127">
+        <v>2.9743001536588398</v>
+      </c>
+      <c r="U127">
+        <v>16.9686307461252</v>
+      </c>
+      <c r="V127">
+        <v>1.8467177992933299</v>
+      </c>
+      <c r="W127">
+        <v>2.4824677838460598</v>
+      </c>
+      <c r="X127">
+        <v>17.684601281331702</v>
+      </c>
+      <c r="Y127">
+        <v>1.4121096824774899</v>
+      </c>
+      <c r="Z127">
+        <v>2.1249155320434898</v>
+      </c>
+      <c r="AA127">
+        <v>0.38018865813311398</v>
+      </c>
+      <c r="AB127">
+        <v>8.5161152493232404</v>
+      </c>
+      <c r="AC127">
+        <v>1.66473905501507</v>
+      </c>
+      <c r="AD127">
+        <v>0.245625329217532</v>
+      </c>
+    </row>
+    <row r="128" spans="1:30" ht="25.5">
+      <c r="A128" s="12"/>
+      <c r="B128" s="12"/>
+      <c r="C128" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D128">
+        <v>31.8</v>
+      </c>
+      <c r="E128">
+        <v>11.180339887498899</v>
+      </c>
+      <c r="F128">
+        <v>2.5240735330017601</v>
+      </c>
+      <c r="G128">
+        <v>0.111840138918903</v>
+      </c>
+      <c r="H128">
+        <v>17.162680658375301</v>
+      </c>
+      <c r="I128">
+        <v>4.5524860269277099</v>
+      </c>
+      <c r="J128">
+        <v>0.46629189514911801</v>
+      </c>
+      <c r="K128">
+        <v>2.62119646498187E-2</v>
+      </c>
+      <c r="L128">
+        <v>8.7641722747500898E-4</v>
+      </c>
+      <c r="M128">
+        <v>1.3737075067236999E-3</v>
+      </c>
+      <c r="N128">
+        <v>8.8892370683818903E-2</v>
+      </c>
+      <c r="O128">
+        <v>5.3081266123910502E-2</v>
+      </c>
+      <c r="P128">
+        <v>34.887094180190303</v>
+      </c>
+      <c r="Q128">
+        <v>0.81754847133651698</v>
+      </c>
+      <c r="R128">
+        <v>4.7574603849127602E-2</v>
+      </c>
+      <c r="S128">
+        <v>4.1242573067102897E-2</v>
+      </c>
+      <c r="T128">
+        <v>2.27790184250772</v>
+      </c>
+      <c r="U128">
+        <v>31.495491345692901</v>
+      </c>
+      <c r="V128">
+        <v>2.4799347877921998E-2</v>
+      </c>
+      <c r="W128">
+        <v>2.8701040610483002E-3</v>
+      </c>
+      <c r="X128">
+        <v>6.5711997479617201</v>
+      </c>
+      <c r="Y128">
+        <v>0.41722175339663198</v>
+      </c>
+      <c r="Z128">
+        <v>5.7930676914654297E-2</v>
+      </c>
+      <c r="AA128" s="10">
+        <v>7.3242642980320504E-5</v>
+      </c>
+      <c r="AB128">
+        <v>0.41019938410927698</v>
+      </c>
+      <c r="AC128">
+        <v>0.36170512656700099</v>
+      </c>
+      <c r="AD128">
+        <v>0.123413154262123</v>
+      </c>
+    </row>
+    <row r="129" spans="1:30" ht="25.5">
+      <c r="A129" s="12"/>
+      <c r="B129" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="130" spans="1:30" ht="25.5">
+      <c r="A130" s="12"/>
+      <c r="B130" s="12"/>
+      <c r="C130" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="133" spans="1:30" ht="25.5">
+      <c r="A133" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B133" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D133">
+        <v>28.279012761000001</v>
+      </c>
+      <c r="E133">
+        <v>16.8331405066271</v>
+      </c>
+      <c r="F133">
+        <v>1.4672848926364099</v>
+      </c>
+      <c r="G133">
+        <v>2.0809491494107202</v>
+      </c>
+      <c r="H133">
+        <v>8.5062398072588099</v>
+      </c>
+      <c r="I133">
+        <v>2.2532302316333301</v>
+      </c>
+      <c r="J133">
+        <v>1.96349807893869</v>
+      </c>
+      <c r="K133">
+        <v>9.4554708085964894</v>
+      </c>
+      <c r="L133">
+        <v>0.65080823814181499</v>
+      </c>
+      <c r="M133">
+        <v>1.76585348228616</v>
+      </c>
+      <c r="N133">
+        <v>8.1194867899248102</v>
+      </c>
+      <c r="O133">
+        <v>3.5208706659477</v>
+      </c>
+      <c r="P133">
+        <v>7.2220401580554698</v>
+      </c>
+      <c r="Q133">
+        <v>0.127862491396452</v>
+      </c>
+      <c r="R133">
+        <v>7.4858477609674603</v>
+      </c>
+      <c r="S133">
+        <v>2.0615733028160501</v>
+      </c>
+      <c r="T133">
+        <v>0.74902983994828298</v>
+      </c>
+      <c r="U133">
+        <v>8.2755987566769402</v>
+      </c>
+      <c r="V133">
+        <v>6.1315713595439796</v>
+      </c>
+      <c r="W133">
+        <v>7.4947289562066599</v>
+      </c>
+      <c r="X133">
+        <v>7.05748992555091</v>
+      </c>
+      <c r="Y133">
+        <v>3.5112682357680698</v>
+      </c>
+      <c r="Z133">
+        <v>0.257178674407048</v>
+      </c>
+      <c r="AA133">
+        <v>1.0892109422982701</v>
+      </c>
+      <c r="AB133">
+        <v>0.54271007347869105</v>
+      </c>
+      <c r="AC133">
+        <v>0.76071014813223503</v>
+      </c>
+      <c r="AD133">
+        <v>8.9167721226148799</v>
+      </c>
+    </row>
+    <row r="134" spans="1:30" ht="25.5">
+      <c r="A134" s="12"/>
+      <c r="B134" s="12"/>
+      <c r="C134" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D134">
+        <v>26.878217083487002</v>
+      </c>
+      <c r="E134">
+        <v>9.9590131889751401</v>
+      </c>
+      <c r="F134">
+        <v>2.33941020474585</v>
+      </c>
+      <c r="G134">
+        <v>10.5785541061713</v>
+      </c>
+      <c r="H134">
+        <v>7.7258772027788301E-3</v>
+      </c>
+      <c r="I134">
+        <v>1.6308903452746999</v>
+      </c>
+      <c r="J134">
+        <v>6.3218438757175397</v>
+      </c>
+      <c r="K134">
+        <v>9.3733262329141507</v>
+      </c>
+      <c r="L134">
+        <v>0.116123865781497</v>
+      </c>
+      <c r="M134">
+        <v>2.1425393871155598</v>
+      </c>
+      <c r="N134">
+        <v>2.8663917593632302</v>
+      </c>
+      <c r="O134">
+        <v>4.5135558091075799E-2</v>
+      </c>
+      <c r="P134">
+        <v>9.8395020425064992</v>
+      </c>
+      <c r="Q134">
+        <v>0.37943276683362698</v>
+      </c>
+      <c r="R134">
+        <v>0.76750864295239396</v>
+      </c>
+      <c r="S134">
+        <v>1.9857351582762399</v>
+      </c>
+      <c r="T134">
+        <v>4.41447824526196</v>
+      </c>
+      <c r="U134">
+        <v>10.451989780894699</v>
+      </c>
+      <c r="V134">
+        <v>6.6184199210071002</v>
+      </c>
+      <c r="W134">
+        <v>8.7993483686005103</v>
+      </c>
+      <c r="X134">
+        <v>5.4272873714929197</v>
+      </c>
+      <c r="Y134">
+        <v>3.3950763001488702</v>
+      </c>
+      <c r="Z134">
+        <v>0.375914997846446</v>
+      </c>
+      <c r="AA134">
+        <v>0.92361440926277805</v>
+      </c>
+      <c r="AB134">
+        <v>8.6950291791008603</v>
+      </c>
+      <c r="AC134">
+        <v>2.82673189507247</v>
+      </c>
+      <c r="AD134">
+        <v>2.0173999131106202</v>
+      </c>
+    </row>
+    <row r="135" spans="1:30" ht="25.5">
+      <c r="A135" s="12"/>
+      <c r="B135" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="136" spans="1:30" ht="25.5">
+      <c r="A136" s="12"/>
+      <c r="B136" s="12"/>
+      <c r="C136" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="137" spans="1:30" ht="25.5">
+      <c r="A137" s="12"/>
+      <c r="B137" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="138" spans="1:30" ht="25.5">
+      <c r="A138" s="12"/>
+      <c r="B138" s="12"/>
+      <c r="C138" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="64">
+  <mergeCells count="72">
     <mergeCell ref="A117:A122"/>
     <mergeCell ref="B117:B118"/>
     <mergeCell ref="B119:B120"/>
@@ -9127,6 +9881,14 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A125:A130"/>
+    <mergeCell ref="B125:B126"/>
+    <mergeCell ref="B127:B128"/>
+    <mergeCell ref="B129:B130"/>
+    <mergeCell ref="A133:A138"/>
+    <mergeCell ref="B133:B134"/>
+    <mergeCell ref="B135:B136"/>
+    <mergeCell ref="B137:B138"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -9172,10 +9934,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -9198,8 +9960,8 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
@@ -9223,10 +9985,10 @@
       <c r="A8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -9249,8 +10011,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="11"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="7" t="s">
         <v>33</v>
       </c>
@@ -9271,10 +10033,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -9282,17 +10044,17 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="11"/>
-      <c r="B13" s="14"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -9315,8 +10077,8 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="11"/>
-      <c r="B16" s="14"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="7" t="s">
         <v>33</v>
       </c>
@@ -9337,10 +10099,10 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -9363,8 +10125,8 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="11"/>
-      <c r="B19" s="14"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="7" t="s">
         <v>33</v>
       </c>
@@ -9385,10 +10147,10 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -9396,17 +10158,17 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="11"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -9429,8 +10191,8 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="11"/>
-      <c r="B25" s="14"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="7" t="s">
         <v>33</v>
       </c>
@@ -9501,10 +10263,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="15" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -9521,8 +10283,8 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="11"/>
-      <c r="B5" s="14"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="7" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
outputs for 22,25,27 ACO and 28,29 MVO outputs and edits
</commit_message>
<xml_diff>
--- a/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
+++ b/OneDrive_2021-09-24/Final Year Project Drive/codes_2022/window-sliding/SlidingWindow_Summary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="63">
   <si>
     <t>Date range</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>27-Jan-2016 ::25-Jan-2021</t>
+  </si>
+  <si>
+    <t>28-Jan-2016 ::27-Jan-2021</t>
+  </si>
+  <si>
+    <t>29-Jan-2016 ::28-Jan-2021</t>
   </si>
 </sst>
 </file>
@@ -703,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMJ138"/>
+  <dimension ref="A1:AMJ154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D136" sqref="D136:AD136"/>
+    <sheetView tabSelected="1" topLeftCell="B137" workbookViewId="0">
+      <selection activeCell="D150" sqref="D150:AD150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -9221,6 +9227,87 @@
       <c r="C121" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="D121">
+        <v>28.879953055551699</v>
+      </c>
+      <c r="E121">
+        <v>17.432115138187399</v>
+      </c>
+      <c r="F121">
+        <v>1.4513415529323099</v>
+      </c>
+      <c r="G121">
+        <v>3.3524590379636101</v>
+      </c>
+      <c r="H121">
+        <v>7.4663502145684904</v>
+      </c>
+      <c r="I121">
+        <v>4.3809318321148298</v>
+      </c>
+      <c r="J121">
+        <v>5.9236410233416601</v>
+      </c>
+      <c r="K121">
+        <v>6.9521138174928803</v>
+      </c>
+      <c r="L121">
+        <v>2.838222640888</v>
+      </c>
+      <c r="M121">
+        <v>3.8666954350392202</v>
+      </c>
+      <c r="N121">
+        <v>4.3809318321148298</v>
+      </c>
+      <c r="O121">
+        <v>0.78127705258556801</v>
+      </c>
+      <c r="P121">
+        <v>7.4663502145684904</v>
+      </c>
+      <c r="Q121">
+        <v>0.78127705258556801</v>
+      </c>
+      <c r="R121">
+        <v>4.8951682291904399</v>
+      </c>
+      <c r="S121">
+        <v>0.78127705258556801</v>
+      </c>
+      <c r="T121">
+        <v>3.8666954350392202</v>
+      </c>
+      <c r="U121">
+        <v>4.3809318321148298</v>
+      </c>
+      <c r="V121">
+        <v>4.3809318321148298</v>
+      </c>
+      <c r="W121">
+        <v>7.9805866116441004</v>
+      </c>
+      <c r="X121">
+        <v>2.3239862438123899</v>
+      </c>
+      <c r="Y121">
+        <v>2.838222640888</v>
+      </c>
+      <c r="Z121">
+        <v>0.78127705258556801</v>
+      </c>
+      <c r="AA121">
+        <v>6.9521138174928803</v>
+      </c>
+      <c r="AB121">
+        <v>7.9805866116441004</v>
+      </c>
+      <c r="AC121">
+        <v>1.29551344966117</v>
+      </c>
+      <c r="AD121">
+        <v>3.3524590379636101</v>
+      </c>
     </row>
     <row r="122" spans="1:30" ht="25.5">
       <c r="A122" s="12"/>
@@ -9228,6 +9315,87 @@
       <c r="C122" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="D122">
+        <v>28.824228508644101</v>
+      </c>
+      <c r="E122">
+        <v>11.0749799486016</v>
+      </c>
+      <c r="F122">
+        <v>2.2793927055219099</v>
+      </c>
+      <c r="G122">
+        <v>5.1568111361917</v>
+      </c>
+      <c r="H122">
+        <v>0.83618072371881602</v>
+      </c>
+      <c r="I122">
+        <v>1.3762595252779199</v>
+      </c>
+      <c r="J122">
+        <v>4.6167323346325899</v>
+      </c>
+      <c r="K122">
+        <v>7.3171263424281401</v>
+      </c>
+      <c r="L122">
+        <v>4.6167323346325899</v>
+      </c>
+      <c r="M122">
+        <v>4.6167323346325899</v>
+      </c>
+      <c r="N122">
+        <v>6.7770475408690301</v>
+      </c>
+      <c r="O122">
+        <v>5.1568111361917</v>
+      </c>
+      <c r="P122">
+        <v>2.9964959299552598</v>
+      </c>
+      <c r="Q122">
+        <v>0.83618072371881602</v>
+      </c>
+      <c r="R122">
+        <v>1.91633832683703</v>
+      </c>
+      <c r="S122">
+        <v>2.4564171283961498</v>
+      </c>
+      <c r="T122">
+        <v>1.3762595252779199</v>
+      </c>
+      <c r="U122">
+        <v>6.23696873930992</v>
+      </c>
+      <c r="V122">
+        <v>1.3762595252779199</v>
+      </c>
+      <c r="W122">
+        <v>6.7770475408690301</v>
+      </c>
+      <c r="X122">
+        <v>8.3972839455463593</v>
+      </c>
+      <c r="Y122">
+        <v>7.8572051439872501</v>
+      </c>
+      <c r="Z122">
+        <v>5.69688993775081</v>
+      </c>
+      <c r="AA122">
+        <v>2.9964959299552598</v>
+      </c>
+      <c r="AB122">
+        <v>7.8572051439872501</v>
+      </c>
+      <c r="AC122">
+        <v>1.3762595252779199</v>
+      </c>
+      <c r="AD122">
+        <v>1.3762595252779199</v>
+      </c>
     </row>
     <row r="125" spans="1:30" ht="25.5">
       <c r="A125" s="11" t="s">
@@ -9595,6 +9763,87 @@
       <c r="C129" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="D129">
+        <v>29.185410202694499</v>
+      </c>
+      <c r="E129">
+        <v>17.778028536487</v>
+      </c>
+      <c r="F129">
+        <v>1.44028400844013</v>
+      </c>
+      <c r="G129">
+        <v>6.5583888473410701</v>
+      </c>
+      <c r="H129">
+        <v>9.0540989489143602</v>
+      </c>
+      <c r="I129">
+        <v>2.19089616958781</v>
+      </c>
+      <c r="J129">
+        <v>1.5669686441944799</v>
+      </c>
+      <c r="K129">
+        <v>5.93446132194775</v>
+      </c>
+      <c r="L129">
+        <v>2.8148236949811301</v>
+      </c>
+      <c r="M129">
+        <v>0.94304111880116304</v>
+      </c>
+      <c r="N129">
+        <v>4.06267874576778</v>
+      </c>
+      <c r="O129">
+        <v>4.6866062711611001</v>
+      </c>
+      <c r="P129">
+        <v>9.0540989489143602</v>
+      </c>
+      <c r="Q129">
+        <v>0.94304111880116304</v>
+      </c>
+      <c r="R129">
+        <v>4.06267874576778</v>
+      </c>
+      <c r="S129">
+        <v>4.6866062711611001</v>
+      </c>
+      <c r="T129">
+        <v>0.94304111880116304</v>
+      </c>
+      <c r="U129">
+        <v>9.6780264743076891</v>
+      </c>
+      <c r="V129">
+        <v>1.5669686441944799</v>
+      </c>
+      <c r="W129">
+        <v>5.93446132194775</v>
+      </c>
+      <c r="X129">
+        <v>8.4301714235210401</v>
+      </c>
+      <c r="Y129">
+        <v>1.5669686441944799</v>
+      </c>
+      <c r="Z129">
+        <v>3.4387512203744501</v>
+      </c>
+      <c r="AA129">
+        <v>2.8148236949811301</v>
+      </c>
+      <c r="AB129">
+        <v>0.94304111880116304</v>
+      </c>
+      <c r="AC129">
+        <v>2.8148236949811301</v>
+      </c>
+      <c r="AD129">
+        <v>5.3105337965544201</v>
+      </c>
     </row>
     <row r="130" spans="1:30" ht="25.5">
       <c r="A130" s="12"/>
@@ -9602,6 +9851,87 @@
       <c r="C130" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="D130">
+        <v>28.968489168101598</v>
+      </c>
+      <c r="E130">
+        <v>11.0041639053875</v>
+      </c>
+      <c r="F130">
+        <v>2.3071711205311698</v>
+      </c>
+      <c r="G130">
+        <v>3.9623391405586301</v>
+      </c>
+      <c r="H130">
+        <v>7.2315795582871596</v>
+      </c>
+      <c r="I130">
+        <v>1.7828455287396101</v>
+      </c>
+      <c r="J130">
+        <v>1.2379721257848499</v>
+      </c>
+      <c r="K130">
+        <v>6.1418327523776499</v>
+      </c>
+      <c r="L130">
+        <v>1.2379721257848499</v>
+      </c>
+      <c r="M130">
+        <v>4.5072125435133801</v>
+      </c>
+      <c r="N130">
+        <v>2.87259233464912</v>
+      </c>
+      <c r="O130">
+        <v>1.2379721257848499</v>
+      </c>
+      <c r="P130">
+        <v>6.6867061553324101</v>
+      </c>
+      <c r="Q130">
+        <v>3.9623391405586301</v>
+      </c>
+      <c r="R130">
+        <v>7.7764529612419198</v>
+      </c>
+      <c r="S130">
+        <v>2.3277189316943598</v>
+      </c>
+      <c r="T130">
+        <v>0.69309872283009999</v>
+      </c>
+      <c r="U130">
+        <v>7.7764529612419198</v>
+      </c>
+      <c r="V130">
+        <v>2.87259233464912</v>
+      </c>
+      <c r="W130">
+        <v>6.6867061553324101</v>
+      </c>
+      <c r="X130">
+        <v>1.2379721257848499</v>
+      </c>
+      <c r="Y130">
+        <v>5.0520859464681402</v>
+      </c>
+      <c r="Z130">
+        <v>2.87259233464912</v>
+      </c>
+      <c r="AA130">
+        <v>2.87259233464912</v>
+      </c>
+      <c r="AB130">
+        <v>8.3213263641966702</v>
+      </c>
+      <c r="AC130">
+        <v>2.87259233464912</v>
+      </c>
+      <c r="AD130">
+        <v>7.7764529612419198</v>
+      </c>
     </row>
     <row r="133" spans="1:30" ht="25.5">
       <c r="A133" s="11" t="s">
@@ -9969,6 +10299,87 @@
       <c r="C137" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="D137">
+        <v>28.831792813462901</v>
+      </c>
+      <c r="E137">
+        <v>18.088853506776498</v>
+      </c>
+      <c r="F137">
+        <v>1.39598636276218</v>
+      </c>
+      <c r="G137">
+        <v>5.6187251714955302</v>
+      </c>
+      <c r="H137">
+        <v>8.3845508949790801</v>
+      </c>
+      <c r="I137">
+        <v>4.51239488210211</v>
+      </c>
+      <c r="J137">
+        <v>3.4060645927086899</v>
+      </c>
+      <c r="K137">
+        <v>4.51239488210211</v>
+      </c>
+      <c r="L137">
+        <v>0.64023886922514195</v>
+      </c>
+      <c r="M137">
+        <v>1.7465691586185601</v>
+      </c>
+      <c r="N137">
+        <v>5.0655600267988197</v>
+      </c>
+      <c r="O137">
+        <v>1.19340401392185</v>
+      </c>
+      <c r="P137">
+        <v>8.3845508949790801</v>
+      </c>
+      <c r="Q137">
+        <v>5.0655600267988197</v>
+      </c>
+      <c r="R137">
+        <v>6.7250554608889397</v>
+      </c>
+      <c r="S137">
+        <v>4.51239488210211</v>
+      </c>
+      <c r="T137">
+        <v>7.8313857502823696</v>
+      </c>
+      <c r="U137">
+        <v>5.6187251714955302</v>
+      </c>
+      <c r="V137">
+        <v>1.19340401392185</v>
+      </c>
+      <c r="W137">
+        <v>7.27822060558566</v>
+      </c>
+      <c r="X137">
+        <v>5.6187251714955302</v>
+      </c>
+      <c r="Y137">
+        <v>4.51239488210211</v>
+      </c>
+      <c r="Z137">
+        <v>0.64023886922514195</v>
+      </c>
+      <c r="AA137">
+        <v>2.2997343033152702</v>
+      </c>
+      <c r="AB137">
+        <v>0.64023886922514195</v>
+      </c>
+      <c r="AC137">
+        <v>2.2997343033152702</v>
+      </c>
+      <c r="AD137">
+        <v>2.2997343033152702</v>
+      </c>
     </row>
     <row r="138" spans="1:30" ht="25.5">
       <c r="A138" s="12"/>
@@ -9976,9 +10387,514 @@
       <c r="C138" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="D138">
+        <v>28.075746940593799</v>
+      </c>
+      <c r="E138">
+        <v>10.7088976947016</v>
+      </c>
+      <c r="F138">
+        <v>2.2874200164143401</v>
+      </c>
+      <c r="G138">
+        <v>4.3448262268312297</v>
+      </c>
+      <c r="H138">
+        <v>3.1231606714170299</v>
+      </c>
+      <c r="I138">
+        <v>1.2906623382957401</v>
+      </c>
+      <c r="J138">
+        <v>8.6206556707809199</v>
+      </c>
+      <c r="K138">
+        <v>8.0098228930738191</v>
+      </c>
+      <c r="L138">
+        <v>1.2906623382957401</v>
+      </c>
+      <c r="M138">
+        <v>4.9556590045383304</v>
+      </c>
+      <c r="N138">
+        <v>7.3989901153667201</v>
+      </c>
+      <c r="O138">
+        <v>1.2906623382957401</v>
+      </c>
+      <c r="P138">
+        <v>9.2314884484880206</v>
+      </c>
+      <c r="Q138">
+        <v>0.67982956058864596</v>
+      </c>
+      <c r="R138">
+        <v>3.1231606714170299</v>
+      </c>
+      <c r="S138">
+        <v>9.2314884484880206</v>
+      </c>
+      <c r="T138">
+        <v>0.67982956058864596</v>
+      </c>
+      <c r="U138">
+        <v>6.1773245599525302</v>
+      </c>
+      <c r="V138">
+        <v>2.5123278937099398</v>
+      </c>
+      <c r="W138">
+        <v>3.1231606714170299</v>
+      </c>
+      <c r="X138">
+        <v>8.6206556707809199</v>
+      </c>
+      <c r="Y138">
+        <v>8.0098228930738191</v>
+      </c>
+      <c r="Z138">
+        <v>1.9014951160028399</v>
+      </c>
+      <c r="AA138">
+        <v>1.9014951160028399</v>
+      </c>
+      <c r="AB138">
+        <v>0.67982956058864596</v>
+      </c>
+      <c r="AC138">
+        <v>1.2906623382957401</v>
+      </c>
+      <c r="AD138">
+        <v>2.5123278937099398</v>
+      </c>
+    </row>
+    <row r="141" spans="1:30" ht="25.5">
+      <c r="A141" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B141" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C141" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D141">
+        <v>31.048160506621901</v>
+      </c>
+      <c r="E141">
+        <v>18.697949380428799</v>
+      </c>
+      <c r="F141">
+        <v>1.46904668248663</v>
+      </c>
+      <c r="G141">
+        <v>7.6785699456160303</v>
+      </c>
+      <c r="H141">
+        <v>10.861913953712101</v>
+      </c>
+      <c r="I141">
+        <v>4.2925236505914501</v>
+      </c>
+      <c r="J141">
+        <v>2.8618134866239702</v>
+      </c>
+      <c r="K141">
+        <v>4.0146161828394202</v>
+      </c>
+      <c r="L141">
+        <v>1.2274781280207301</v>
+      </c>
+      <c r="M141">
+        <v>3.4065760178950701</v>
+      </c>
+      <c r="N141">
+        <v>4.2967945715095199</v>
+      </c>
+      <c r="O141">
+        <v>5.4319097939441798</v>
+      </c>
+      <c r="P141">
+        <v>10.4768036241878</v>
+      </c>
+      <c r="Q141">
+        <v>0.23790082170861401</v>
+      </c>
+      <c r="R141">
+        <v>3.5117143479375401</v>
+      </c>
+      <c r="S141">
+        <v>3.52517755679873</v>
+      </c>
+      <c r="T141">
+        <v>2.1328325034439501</v>
+      </c>
+      <c r="U141">
+        <v>3.4273878833355602</v>
+      </c>
+      <c r="V141">
+        <v>5.6026403554339903E-2</v>
+      </c>
+      <c r="W141">
+        <v>1.20001255457504</v>
+      </c>
+      <c r="X141">
+        <v>9.9313229332774799</v>
+      </c>
+      <c r="Y141">
+        <v>6.5487529030751599</v>
+      </c>
+      <c r="Z141">
+        <v>1.02251627495349</v>
+      </c>
+      <c r="AA141">
+        <v>2.8631162117386899</v>
+      </c>
+      <c r="AB141">
+        <v>10.040776942640701</v>
+      </c>
+      <c r="AC141">
+        <v>0.20491518276145601</v>
+      </c>
+      <c r="AD141">
+        <v>0.74854812525875503</v>
+      </c>
+    </row>
+    <row r="142" spans="1:30" ht="25.5">
+      <c r="A142" s="12"/>
+      <c r="B142" s="12"/>
+      <c r="C142" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D142">
+        <v>29.894563164898901</v>
+      </c>
+      <c r="E142">
+        <v>11.3109013373178</v>
+      </c>
+      <c r="F142">
+        <v>2.3264780038421602</v>
+      </c>
+      <c r="G142">
+        <v>3.7632624491503899</v>
+      </c>
+      <c r="H142">
+        <v>6.9642569165450698</v>
+      </c>
+      <c r="I142">
+        <v>9.9855360127929202</v>
+      </c>
+      <c r="J142">
+        <v>7.41085622494374</v>
+      </c>
+      <c r="K142">
+        <v>8.1809350697252601</v>
+      </c>
+      <c r="L142">
+        <v>1.86415521561727</v>
+      </c>
+      <c r="M142">
+        <v>0.463928116024382</v>
+      </c>
+      <c r="N142">
+        <v>5.7687975245332099</v>
+      </c>
+      <c r="O142">
+        <v>0.89514579762486302</v>
+      </c>
+      <c r="P142">
+        <v>10.0689418526135</v>
+      </c>
+      <c r="Q142">
+        <v>1.4899012529142699</v>
+      </c>
+      <c r="R142">
+        <v>4.8729514574073898</v>
+      </c>
+      <c r="S142">
+        <v>2.86440744338528</v>
+      </c>
+      <c r="T142">
+        <v>0.40960481504548502</v>
+      </c>
+      <c r="U142">
+        <v>11.0530610219802</v>
+      </c>
+      <c r="V142">
+        <v>1.92843965337704</v>
+      </c>
+      <c r="W142">
+        <v>1.38116275591674E-2</v>
+      </c>
+      <c r="X142">
+        <v>4.7104521832492097</v>
+      </c>
+      <c r="Y142">
+        <v>2.37915257622201</v>
+      </c>
+      <c r="Z142">
+        <v>0.69739887255963395</v>
+      </c>
+      <c r="AA142">
+        <v>0.71528213316108702</v>
+      </c>
+      <c r="AB142">
+        <v>9.9618442949038197</v>
+      </c>
+      <c r="AC142">
+        <v>1.74215051684276</v>
+      </c>
+      <c r="AD142">
+        <v>1.79572697182184</v>
+      </c>
+    </row>
+    <row r="143" spans="1:30" ht="25.5">
+      <c r="A143" s="12"/>
+      <c r="B143" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C143" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="144" spans="1:30" ht="25.5">
+      <c r="A144" s="12"/>
+      <c r="B144" s="12"/>
+      <c r="C144" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="145" spans="1:30" ht="25.5">
+      <c r="A145" s="12"/>
+      <c r="B145" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="146" spans="1:30" ht="25.5">
+      <c r="A146" s="12"/>
+      <c r="B146" s="12"/>
+      <c r="C146" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="149" spans="1:30" ht="25.5">
+      <c r="A149" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B149" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C149" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D149">
+        <v>29.0033733162673</v>
+      </c>
+      <c r="E149">
+        <v>17.6684103777018</v>
+      </c>
+      <c r="F149">
+        <v>1.4389168449671399</v>
+      </c>
+      <c r="G149">
+        <v>8.4941639037863101</v>
+      </c>
+      <c r="H149">
+        <v>7.78784650118883</v>
+      </c>
+      <c r="I149">
+        <v>6.4288009907120598</v>
+      </c>
+      <c r="J149">
+        <v>8.3785403807861094</v>
+      </c>
+      <c r="K149">
+        <v>5.6745391956949103</v>
+      </c>
+      <c r="L149">
+        <v>0.74745933145186305</v>
+      </c>
+      <c r="M149">
+        <v>2.12276300595643</v>
+      </c>
+      <c r="N149">
+        <v>1.18498916874866</v>
+      </c>
+      <c r="O149">
+        <v>1.9548882228353901</v>
+      </c>
+      <c r="P149">
+        <v>7.0433845890905404</v>
+      </c>
+      <c r="Q149">
+        <v>0.60193230926021901</v>
+      </c>
+      <c r="R149">
+        <v>4.6759433919544398</v>
+      </c>
+      <c r="S149">
+        <v>0.43712332962118799</v>
+      </c>
+      <c r="T149">
+        <v>0.53253685824388697</v>
+      </c>
+      <c r="U149">
+        <v>5.8189712306670502</v>
+      </c>
+      <c r="V149">
+        <v>3.65153834274131</v>
+      </c>
+      <c r="W149">
+        <v>5.9875467012085997</v>
+      </c>
+      <c r="X149">
+        <v>8.2899257774099695</v>
+      </c>
+      <c r="Y149">
+        <v>7.7125303059791497</v>
+      </c>
+      <c r="Z149">
+        <v>0.427307532726865</v>
+      </c>
+      <c r="AA149">
+        <v>4.6158580705315497</v>
+      </c>
+      <c r="AB149">
+        <v>5.4085829341973204</v>
+      </c>
+      <c r="AC149">
+        <v>0.64563277536275099</v>
+      </c>
+      <c r="AD149">
+        <v>1.3771951498445101</v>
+      </c>
+    </row>
+    <row r="150" spans="1:30" ht="25.5">
+      <c r="A150" s="12"/>
+      <c r="B150" s="12"/>
+      <c r="C150" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D150">
+        <v>29.449503903422801</v>
+      </c>
+      <c r="E150">
+        <v>11.3669398837446</v>
+      </c>
+      <c r="F150">
+        <v>2.2758547302970702</v>
+      </c>
+      <c r="G150">
+        <v>1.91135119545141</v>
+      </c>
+      <c r="H150">
+        <v>8.7159404544612595</v>
+      </c>
+      <c r="I150">
+        <v>1.21827080206764</v>
+      </c>
+      <c r="J150">
+        <v>8.2586150457964305</v>
+      </c>
+      <c r="K150">
+        <v>3.7693095036965398</v>
+      </c>
+      <c r="L150">
+        <v>1.3364824109470901</v>
+      </c>
+      <c r="M150">
+        <v>1.0262890806492699</v>
+      </c>
+      <c r="N150">
+        <v>3.0791478633563898</v>
+      </c>
+      <c r="O150">
+        <v>2.5200926183614598</v>
+      </c>
+      <c r="P150">
+        <v>6.7136609527052</v>
+      </c>
+      <c r="Q150">
+        <v>1.2134003140424701</v>
+      </c>
+      <c r="R150">
+        <v>0.603823961115034</v>
+      </c>
+      <c r="S150">
+        <v>2.68956994095559</v>
+      </c>
+      <c r="T150">
+        <v>0.80874273355994297</v>
+      </c>
+      <c r="U150">
+        <v>8.55915281671248</v>
+      </c>
+      <c r="V150">
+        <v>1.6154273854061301</v>
+      </c>
+      <c r="W150">
+        <v>9.9164524725486203</v>
+      </c>
+      <c r="X150">
+        <v>7.1044370858483203</v>
+      </c>
+      <c r="Y150">
+        <v>5.47567598991722</v>
+      </c>
+      <c r="Z150">
+        <v>7.7832523664216096</v>
+      </c>
+      <c r="AA150">
+        <v>3.7219310652836999</v>
+      </c>
+      <c r="AB150">
+        <v>7.5641390168057301</v>
+      </c>
+      <c r="AC150">
+        <v>0.43321488256406099</v>
+      </c>
+      <c r="AD150">
+        <v>3.9616200413263201</v>
+      </c>
+    </row>
+    <row r="151" spans="1:30" ht="25.5">
+      <c r="A151" s="12"/>
+      <c r="B151" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C151" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="152" spans="1:30" ht="25.5">
+      <c r="A152" s="12"/>
+      <c r="B152" s="12"/>
+      <c r="C152" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="153" spans="1:30" ht="25.5">
+      <c r="A153" s="12"/>
+      <c r="B153" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="154" spans="1:30" ht="25.5">
+      <c r="A154" s="12"/>
+      <c r="B154" s="12"/>
+      <c r="C154" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="72">
+  <mergeCells count="80">
     <mergeCell ref="A125:A130"/>
     <mergeCell ref="B125:B126"/>
     <mergeCell ref="B127:B128"/>
@@ -10051,6 +10967,14 @@
     <mergeCell ref="B109:B110"/>
     <mergeCell ref="B111:B112"/>
     <mergeCell ref="B113:B114"/>
+    <mergeCell ref="A141:A146"/>
+    <mergeCell ref="B141:B142"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="A149:A154"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="B151:B152"/>
+    <mergeCell ref="B153:B154"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>